<commit_message>
Adjusted file detection to be universal (to avoid file location errors), added classroom building for constraint checkin
</commit_message>
<xml_diff>
--- a/data/Timetable_Input_Template.xlsx
+++ b/data/Timetable_Input_Template.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20417"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AL-HAMEEN\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jamil\Downloads\Timetable Scheduler Github\PAU_Timetable_Scheduler\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAD6B69F-DE5E-41CA-8A8F-6F7FCBCA057C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11385" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11388" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Classrooms" sheetId="1" r:id="rId1"/>
@@ -18,14 +19,14 @@
     <sheet name="Courses" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Courses!$J$1:$J$153</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Courses!$J$1:$J$154</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2048" uniqueCount="739">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2056" uniqueCount="740">
   <si>
     <t>Room Name</t>
   </si>
@@ -2242,18 +2243,28 @@
   </si>
   <si>
     <t>Faculty Name</t>
+  </si>
+  <si>
+    <t>PAU-CSC 111</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2348,41 +2359,44 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -2687,20 +2701,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" customWidth="1"/>
-    <col min="2" max="2" width="8.28515625" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" customWidth="1"/>
-    <col min="4" max="4" width="36.42578125" customWidth="1"/>
-    <col min="5" max="5" width="14.5703125" customWidth="1"/>
+    <col min="1" max="1" width="15.33203125" customWidth="1"/>
+    <col min="2" max="2" width="8.33203125" customWidth="1"/>
+    <col min="3" max="3" width="8.6640625" customWidth="1"/>
+    <col min="4" max="4" width="36.44140625" customWidth="1"/>
+    <col min="5" max="5" width="14.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -2740,7 +2754,7 @@
         <v>5</v>
       </c>
       <c r="C3">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="D3" t="s">
         <v>8</v>
@@ -3271,13 +3285,13 @@
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B17 B18:B22 B23:B24 B25:B40 B41:B1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B17 B18:B22 B23:B24 B25:B40 B41:B1048576" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"SST, TYD"</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C23 C24:C34 C35:C1048576">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C23 C24:C34 C35:C1048576" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D23 D24:D40 D41:D1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D23 D24:D40 D41:D1048576" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"Classroom, Phy Lab, Chem Lab, Hall, Workshop, Comp Lab, Fluid Mech Lab, Mechanics Lab, Materials Lab, Thermo Lab, Studio"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3290,23 +3304,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I111"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="30.42578125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="26.7109375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="30.44140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="26.6640625" style="2" customWidth="1"/>
     <col min="3" max="3" width="34" style="2" customWidth="1"/>
     <col min="4" max="4" width="12" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="6" width="22.28515625" customWidth="1"/>
-    <col min="7" max="8" width="14.5703125" customWidth="1"/>
-    <col min="9" max="9" width="11.85546875" customWidth="1"/>
+    <col min="6" max="6" width="22.33203125" customWidth="1"/>
+    <col min="7" max="8" width="14.5546875" customWidth="1"/>
+    <col min="9" max="9" width="11.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -5527,20 +5541,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="9.140625" customWidth="1"/>
-    <col min="2" max="2" width="28.7109375" customWidth="1"/>
-    <col min="3" max="3" width="6.42578125" customWidth="1"/>
-    <col min="4" max="4" width="19.140625" customWidth="1"/>
-    <col min="5" max="5" width="9.28515625" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" customWidth="1"/>
+    <col min="2" max="2" width="28.6640625" customWidth="1"/>
+    <col min="3" max="3" width="6.44140625" customWidth="1"/>
+    <col min="4" max="4" width="19.109375" customWidth="1"/>
+    <col min="5" max="5" width="9.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -6497,10 +6511,10 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1048576" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>"100, 200, 300, 400, 500"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{00000000-0002-0000-0200-000001000000}">
       <formula1>"Electrical Engineering, Mechanical Engineering, Finance, Mechatronics Engineering, Software Engineering, IOH, Economics, Business Administration, Accounting, Mass Communication, ISMS, Film &amp; Media Studies, Computer Science"</formula1>
     </dataValidation>
   </dataValidations>
@@ -6509,25 +6523,25 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K149"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:K150"/>
   <sheetViews>
-    <sheetView topLeftCell="A138" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H138" sqref="H138"/>
+    <sheetView topLeftCell="A2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="14.140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="61.28515625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="26.28515625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="28.28515625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="30.42578125" style="2" customWidth="1"/>
-    <col min="7" max="8" width="30.7109375" style="2" customWidth="1"/>
-    <col min="9" max="9" width="16.140625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="14.109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="61.33203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="26.33203125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="28.33203125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="30.44140625" style="2" customWidth="1"/>
+    <col min="7" max="8" width="30.6640625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="16.109375" style="2" customWidth="1"/>
     <col min="10" max="10" width="34" style="2" customWidth="1"/>
-    <col min="11" max="11" width="20.7109375" customWidth="1"/>
+    <col min="11" max="11" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1">
@@ -7004,27 +7018,27 @@
     </row>
     <row r="16" spans="1:11">
       <c r="A16" s="2" t="s">
-        <v>447</v>
+        <v>739</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>448</v>
+        <v>599</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>449</v>
+        <v>419</v>
       </c>
       <c r="D16" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>85</v>
+        <v>600</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>335</v>
       </c>
-      <c r="H16" s="12" t="s">
+      <c r="H16" s="14" t="s">
         <v>337</v>
       </c>
       <c r="J16" s="2" t="s">
@@ -7033,22 +7047,22 @@
     </row>
     <row r="17" spans="1:10">
       <c r="A17" s="2" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>419</v>
+        <v>449</v>
       </c>
       <c r="D17" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>335</v>
@@ -7062,22 +7076,22 @@
     </row>
     <row r="18" spans="1:10">
       <c r="A18" s="2" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>419</v>
       </c>
       <c r="D18" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>335</v>
@@ -7091,28 +7105,28 @@
     </row>
     <row r="19" spans="1:10">
       <c r="A19" s="2" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>419</v>
       </c>
       <c r="D19" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="G19" s="12" t="s">
-        <v>343</v>
+        <v>89</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>335</v>
       </c>
       <c r="H19" s="12" t="s">
-        <v>345</v>
+        <v>337</v>
       </c>
       <c r="J19" s="2" t="s">
         <v>82</v>
@@ -7120,10 +7134,10 @@
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="2" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>419</v>
@@ -7135,7 +7149,7 @@
         <v>6</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="G20" s="12" t="s">
         <v>343</v>
@@ -7149,22 +7163,22 @@
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="2" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>419</v>
       </c>
       <c r="D21" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="G21" s="12" t="s">
         <v>343</v>
@@ -7178,10 +7192,10 @@
     </row>
     <row r="22" spans="1:10">
       <c r="A22" s="2" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>419</v>
@@ -7193,7 +7207,7 @@
         <v>6</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G22" s="12" t="s">
         <v>343</v>
@@ -7207,16 +7221,16 @@
     </row>
     <row r="23" spans="1:10">
       <c r="A23" s="2" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>419</v>
       </c>
       <c r="D23" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>6</v>
@@ -7236,10 +7250,10 @@
     </row>
     <row r="24" spans="1:10">
       <c r="A24" s="2" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>419</v>
@@ -7251,7 +7265,7 @@
         <v>6</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G24" s="12" t="s">
         <v>343</v>
@@ -7265,10 +7279,10 @@
     </row>
     <row r="25" spans="1:10">
       <c r="A25" s="2" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>419</v>
@@ -7280,7 +7294,7 @@
         <v>6</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="G25" s="12" t="s">
         <v>343</v>
@@ -7294,10 +7308,10 @@
     </row>
     <row r="26" spans="1:10">
       <c r="A26" s="2" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>419</v>
@@ -7309,27 +7323,24 @@
         <v>6</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G26" s="12" t="s">
-        <v>392</v>
-      </c>
-      <c r="H26" s="2" t="s">
-        <v>367</v>
-      </c>
-      <c r="I26" s="2" t="s">
-        <v>359</v>
+        <v>343</v>
+      </c>
+      <c r="H26" s="12" t="s">
+        <v>345</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>103</v>
+        <v>82</v>
       </c>
     </row>
     <row r="27" spans="1:10">
       <c r="A27" s="2" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>419</v>
@@ -7341,21 +7352,27 @@
         <v>6</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>61</v>
+        <v>101</v>
       </c>
       <c r="G27" s="12" t="s">
         <v>392</v>
       </c>
+      <c r="H27" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>359</v>
+      </c>
       <c r="J27" s="2" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="28" spans="1:10">
       <c r="A28" s="2" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>419</v>
@@ -7367,7 +7384,7 @@
         <v>6</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>104</v>
+        <v>61</v>
       </c>
       <c r="G28" s="12" t="s">
         <v>392</v>
@@ -7378,16 +7395,16 @@
     </row>
     <row r="29" spans="1:10">
       <c r="A29" s="2" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>419</v>
       </c>
       <c r="D29" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>6</v>
@@ -7404,25 +7421,25 @@
     </row>
     <row r="30" spans="1:10">
       <c r="A30" s="2" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>419</v>
       </c>
       <c r="D30" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="G30" s="12" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="J30" s="2" t="s">
         <v>103</v>
@@ -7430,10 +7447,10 @@
     </row>
     <row r="31" spans="1:10">
       <c r="A31" s="2" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>419</v>
@@ -7445,7 +7462,7 @@
         <v>6</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>54</v>
+        <v>108</v>
       </c>
       <c r="G31" s="12" t="s">
         <v>395</v>
@@ -7456,10 +7473,10 @@
     </row>
     <row r="32" spans="1:10">
       <c r="A32" s="2" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>419</v>
@@ -7471,7 +7488,7 @@
         <v>6</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>110</v>
+        <v>54</v>
       </c>
       <c r="G32" s="12" t="s">
         <v>395</v>
@@ -7482,22 +7499,22 @@
     </row>
     <row r="33" spans="1:10">
       <c r="A33" s="2" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>419</v>
       </c>
       <c r="D33" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="G33" s="12" t="s">
         <v>395</v>
@@ -7508,22 +7525,22 @@
     </row>
     <row r="34" spans="1:10">
       <c r="A34" s="2" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>419</v>
       </c>
       <c r="D34" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="G34" s="12" t="s">
         <v>395</v>
@@ -7534,10 +7551,10 @@
     </row>
     <row r="35" spans="1:10">
       <c r="A35" s="2" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>419</v>
@@ -7549,27 +7566,21 @@
         <v>6</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="G35" s="12" t="s">
         <v>395</v>
       </c>
-      <c r="H35" s="12" t="s">
-        <v>369</v>
-      </c>
-      <c r="I35" s="12" t="s">
-        <v>361</v>
-      </c>
       <c r="J35" s="2" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="36" spans="1:10">
       <c r="A36" s="2" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>419</v>
@@ -7581,7 +7592,7 @@
         <v>6</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="G36" s="12" t="s">
         <v>395</v>
@@ -7598,10 +7609,10 @@
     </row>
     <row r="37" spans="1:10">
       <c r="A37" s="2" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>419</v>
@@ -7613,39 +7624,45 @@
         <v>6</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="G37" s="2" t="s">
-        <v>359</v>
-      </c>
-      <c r="H37" s="2" t="s">
-        <v>351</v>
+        <v>117</v>
+      </c>
+      <c r="G37" s="12" t="s">
+        <v>395</v>
+      </c>
+      <c r="H37" s="12" t="s">
+        <v>369</v>
+      </c>
+      <c r="I37" s="12" t="s">
+        <v>361</v>
       </c>
       <c r="J37" s="2" t="s">
-        <v>121</v>
+        <v>103</v>
       </c>
     </row>
     <row r="38" spans="1:10">
       <c r="A38" s="2" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>419</v>
       </c>
       <c r="D38" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>375</v>
+        <v>359</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>351</v>
       </c>
       <c r="J38" s="2" t="s">
         <v>121</v>
@@ -7653,10 +7670,10 @@
     </row>
     <row r="39" spans="1:10">
       <c r="A39" s="2" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>419</v>
@@ -7668,7 +7685,7 @@
         <v>14</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>496</v>
+        <v>122</v>
       </c>
       <c r="G39" s="2" t="s">
         <v>375</v>
@@ -7679,25 +7696,25 @@
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="2" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>419</v>
       </c>
       <c r="D40" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="G40" s="12" t="s">
-        <v>382</v>
+        <v>496</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>375</v>
       </c>
       <c r="J40" s="2" t="s">
         <v>121</v>
@@ -7705,22 +7722,22 @@
     </row>
     <row r="41" spans="1:10">
       <c r="A41" s="2" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>419</v>
       </c>
       <c r="D41" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E41" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="G41" s="12" t="s">
         <v>382</v>
@@ -7731,10 +7748,10 @@
     </row>
     <row r="42" spans="1:10">
       <c r="A42" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>419</v>
@@ -7743,10 +7760,10 @@
         <v>3</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="G42" s="12" t="s">
         <v>382</v>
@@ -7757,22 +7774,22 @@
     </row>
     <row r="43" spans="1:10">
       <c r="A43" s="2" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>449</v>
+        <v>419</v>
       </c>
       <c r="D43" s="2">
         <v>3</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="G43" s="12" t="s">
         <v>382</v>
@@ -7783,22 +7800,22 @@
     </row>
     <row r="44" spans="1:10">
       <c r="A44" s="2" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>419</v>
+        <v>449</v>
       </c>
       <c r="D44" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E44" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>122</v>
+        <v>129</v>
       </c>
       <c r="G44" s="12" t="s">
         <v>382</v>
@@ -7809,22 +7826,22 @@
     </row>
     <row r="45" spans="1:10">
       <c r="A45" s="2" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>449</v>
+        <v>419</v>
       </c>
       <c r="D45" s="2">
         <v>2</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F45" s="13" t="s">
-        <v>131</v>
+        <v>6</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>122</v>
       </c>
       <c r="G45" s="12" t="s">
         <v>382</v>
@@ -7835,13 +7852,13 @@
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="2" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>419</v>
+        <v>449</v>
       </c>
       <c r="D46" s="2">
         <v>2</v>
@@ -7849,8 +7866,8 @@
       <c r="E46" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F46" s="2" t="s">
-        <v>133</v>
+      <c r="F46" s="13" t="s">
+        <v>131</v>
       </c>
       <c r="G46" s="12" t="s">
         <v>382</v>
@@ -7861,10 +7878,10 @@
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="2" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>419</v>
@@ -7873,24 +7890,24 @@
         <v>2</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="G47" s="12" t="s">
-        <v>359</v>
+        <v>382</v>
       </c>
       <c r="J47" s="2" t="s">
-        <v>137</v>
+        <v>121</v>
       </c>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="2" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>419</v>
@@ -7902,27 +7919,21 @@
         <v>6</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="G48" s="12" t="s">
         <v>359</v>
       </c>
-      <c r="H48" s="2" t="s">
-        <v>367</v>
-      </c>
-      <c r="I48" s="2" t="s">
-        <v>401</v>
-      </c>
       <c r="J48" s="2" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="49" spans="1:10">
       <c r="A49" s="2" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>419</v>
@@ -7934,7 +7945,7 @@
         <v>6</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>517</v>
+        <v>140</v>
       </c>
       <c r="G49" s="12" t="s">
         <v>359</v>
@@ -7951,10 +7962,10 @@
     </row>
     <row r="50" spans="1:10">
       <c r="A50" s="2" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>419</v>
@@ -7966,15 +7977,15 @@
         <v>6</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>146</v>
+        <v>517</v>
       </c>
       <c r="G50" s="12" t="s">
         <v>359</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>351</v>
-      </c>
-      <c r="I50" s="12" t="s">
+        <v>367</v>
+      </c>
+      <c r="I50" s="2" t="s">
         <v>401</v>
       </c>
       <c r="J50" s="2" t="s">
@@ -7983,25 +7994,31 @@
     </row>
     <row r="51" spans="1:10">
       <c r="A51" s="2" t="s">
-        <v>556</v>
+        <v>518</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>557</v>
+        <v>519</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>419</v>
       </c>
       <c r="D51" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E51" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="G51" s="2" t="s">
-        <v>363</v>
+        <v>146</v>
+      </c>
+      <c r="G51" s="12" t="s">
+        <v>359</v>
+      </c>
+      <c r="H51" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="I51" s="12" t="s">
+        <v>401</v>
       </c>
       <c r="J51" s="2" t="s">
         <v>137</v>
@@ -8009,10 +8026,10 @@
     </row>
     <row r="52" spans="1:10">
       <c r="A52" s="2" t="s">
-        <v>520</v>
+        <v>556</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>521</v>
+        <v>557</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>419</v>
@@ -8024,7 +8041,7 @@
         <v>6</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>522</v>
+        <v>152</v>
       </c>
       <c r="G52" s="2" t="s">
         <v>363</v>
@@ -8035,13 +8052,13 @@
     </row>
     <row r="53" spans="1:10">
       <c r="A53" s="2" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>449</v>
+        <v>419</v>
       </c>
       <c r="D53" s="2">
         <v>3</v>
@@ -8049,8 +8066,11 @@
       <c r="E53" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G53" s="12" t="s">
-        <v>365</v>
+      <c r="F53" s="2" t="s">
+        <v>522</v>
+      </c>
+      <c r="G53" s="2" t="s">
+        <v>363</v>
       </c>
       <c r="J53" s="2" t="s">
         <v>137</v>
@@ -8061,10 +8081,10 @@
         <v>523</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>419</v>
+        <v>449</v>
       </c>
       <c r="D54" s="2">
         <v>3</v>
@@ -8072,9 +8092,6 @@
       <c r="E54" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F54" s="2" t="s">
-        <v>150</v>
-      </c>
       <c r="G54" s="12" t="s">
         <v>365</v>
       </c>
@@ -8084,10 +8101,10 @@
     </row>
     <row r="55" spans="1:10">
       <c r="A55" s="2" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>419</v>
@@ -8099,7 +8116,7 @@
         <v>6</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>138</v>
+        <v>150</v>
       </c>
       <c r="G55" s="12" t="s">
         <v>365</v>
@@ -8110,10 +8127,10 @@
     </row>
     <row r="56" spans="1:10">
       <c r="A56" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>419</v>
@@ -8125,7 +8142,7 @@
         <v>6</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>150</v>
+        <v>138</v>
       </c>
       <c r="G56" s="12" t="s">
         <v>365</v>
@@ -8136,10 +8153,10 @@
     </row>
     <row r="57" spans="1:10">
       <c r="A57" s="2" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>419</v>
@@ -8151,7 +8168,7 @@
         <v>6</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="G57" s="12" t="s">
         <v>365</v>
@@ -8162,10 +8179,10 @@
     </row>
     <row r="58" spans="1:10">
       <c r="A58" s="2" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>419</v>
@@ -8177,7 +8194,7 @@
         <v>6</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="G58" s="12" t="s">
         <v>365</v>
@@ -8188,10 +8205,10 @@
     </row>
     <row r="59" spans="1:10">
       <c r="A59" s="2" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="C59" s="2" t="s">
         <v>419</v>
@@ -8203,7 +8220,7 @@
         <v>6</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G59" s="12" t="s">
         <v>365</v>
@@ -8214,36 +8231,36 @@
     </row>
     <row r="60" spans="1:10">
       <c r="A60" s="2" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="C60" s="2" t="s">
         <v>419</v>
       </c>
       <c r="D60" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E60" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="G60" s="12" t="s">
-        <v>351</v>
+        <v>365</v>
       </c>
       <c r="J60" s="2" t="s">
-        <v>160</v>
+        <v>137</v>
       </c>
     </row>
     <row r="61" spans="1:10">
       <c r="A61" s="2" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>419</v>
@@ -8255,7 +8272,7 @@
         <v>6</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="G61" s="12" t="s">
         <v>351</v>
@@ -8266,51 +8283,48 @@
     </row>
     <row r="62" spans="1:10">
       <c r="A62" s="2" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="C62" s="2" t="s">
         <v>419</v>
       </c>
       <c r="D62" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E62" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="G62" s="12" t="s">
         <v>351</v>
       </c>
-      <c r="H62" s="2" t="s">
-        <v>373</v>
-      </c>
       <c r="J62" s="2" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="63" spans="1:10">
       <c r="A63" s="2" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="C63" s="2" t="s">
         <v>419</v>
       </c>
       <c r="D63" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E63" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="G63" s="12" t="s">
         <v>351</v>
@@ -8324,22 +8338,28 @@
     </row>
     <row r="64" spans="1:10">
       <c r="A64" s="2" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>449</v>
+        <v>419</v>
       </c>
       <c r="D64" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E64" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="F64" s="2" t="s">
+        <v>167</v>
+      </c>
       <c r="G64" s="12" t="s">
-        <v>355</v>
+        <v>351</v>
+      </c>
+      <c r="H64" s="2" t="s">
+        <v>373</v>
       </c>
       <c r="J64" s="2" t="s">
         <v>160</v>
@@ -8347,13 +8367,13 @@
     </row>
     <row r="65" spans="1:10">
       <c r="A65" s="2" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>419</v>
+        <v>449</v>
       </c>
       <c r="D65" s="2">
         <v>3</v>
@@ -8361,11 +8381,8 @@
       <c r="E65" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F65" s="2" t="s">
-        <v>144</v>
-      </c>
       <c r="G65" s="12" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="J65" s="2" t="s">
         <v>160</v>
@@ -8373,10 +8390,10 @@
     </row>
     <row r="66" spans="1:10">
       <c r="A66" s="2" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="C66" s="2" t="s">
         <v>419</v>
@@ -8388,7 +8405,7 @@
         <v>6</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="G66" s="12" t="s">
         <v>357</v>
@@ -8399,10 +8416,10 @@
     </row>
     <row r="67" spans="1:10">
       <c r="A67" s="2" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="C67" s="2" t="s">
         <v>419</v>
@@ -8414,7 +8431,7 @@
         <v>6</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>169</v>
+        <v>142</v>
       </c>
       <c r="G67" s="12" t="s">
         <v>357</v>
@@ -8425,22 +8442,22 @@
     </row>
     <row r="68" spans="1:10">
       <c r="A68" s="2" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="C68" s="2" t="s">
         <v>419</v>
       </c>
       <c r="D68" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E68" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>142</v>
+        <v>169</v>
       </c>
       <c r="G68" s="12" t="s">
         <v>357</v>
@@ -8451,10 +8468,10 @@
     </row>
     <row r="69" spans="1:10">
       <c r="A69" s="2" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="C69" s="2" t="s">
         <v>419</v>
@@ -8466,7 +8483,7 @@
         <v>6</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>161</v>
+        <v>142</v>
       </c>
       <c r="G69" s="12" t="s">
         <v>357</v>
@@ -8477,10 +8494,10 @@
     </row>
     <row r="70" spans="1:10">
       <c r="A70" s="2" t="s">
-        <v>558</v>
+        <v>554</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
       <c r="C70" s="2" t="s">
         <v>419</v>
@@ -8492,10 +8509,10 @@
         <v>6</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="G70" s="12" t="s">
-        <v>407</v>
+        <v>357</v>
       </c>
       <c r="J70" s="2" t="s">
         <v>160</v>
@@ -8503,36 +8520,36 @@
     </row>
     <row r="71" spans="1:10">
       <c r="A71" s="2" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="C71" s="2" t="s">
         <v>419</v>
       </c>
       <c r="D71" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E71" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="G71" s="12" t="s">
-        <v>367</v>
+        <v>407</v>
       </c>
       <c r="J71" s="2" t="s">
-        <v>173</v>
+        <v>160</v>
       </c>
     </row>
     <row r="72" spans="1:10">
       <c r="A72" s="2" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="C72" s="2" t="s">
         <v>419</v>
@@ -8544,10 +8561,10 @@
         <v>6</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="G72" s="2" t="s">
-        <v>373</v>
+        <v>176</v>
+      </c>
+      <c r="G72" s="12" t="s">
+        <v>367</v>
       </c>
       <c r="J72" s="2" t="s">
         <v>173</v>
@@ -8555,10 +8572,10 @@
     </row>
     <row r="73" spans="1:10">
       <c r="A73" s="2" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="C73" s="2" t="s">
         <v>419</v>
@@ -8570,7 +8587,7 @@
         <v>6</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="G73" s="2" t="s">
         <v>373</v>
@@ -8581,10 +8598,10 @@
     </row>
     <row r="74" spans="1:10">
       <c r="A74" s="2" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="C74" s="2" t="s">
         <v>419</v>
@@ -8596,7 +8613,7 @@
         <v>6</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="G74" s="2" t="s">
         <v>373</v>
@@ -8607,10 +8624,10 @@
     </row>
     <row r="75" spans="1:10">
       <c r="A75" s="2" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="C75" s="2" t="s">
         <v>419</v>
@@ -8622,7 +8639,7 @@
         <v>6</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="G75" s="2" t="s">
         <v>373</v>
@@ -8633,10 +8650,10 @@
     </row>
     <row r="76" spans="1:10">
       <c r="A76" s="2" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="C76" s="2" t="s">
         <v>419</v>
@@ -8648,21 +8665,21 @@
         <v>6</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="G76" s="2" t="s">
-        <v>401</v>
+        <v>373</v>
       </c>
       <c r="J76" s="2" t="s">
-        <v>188</v>
+        <v>173</v>
       </c>
     </row>
     <row r="77" spans="1:10">
       <c r="A77" s="2" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="C77" s="2" t="s">
         <v>419</v>
@@ -8674,10 +8691,10 @@
         <v>6</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="G77" s="12" t="s">
-        <v>403</v>
+        <v>193</v>
+      </c>
+      <c r="G77" s="2" t="s">
+        <v>401</v>
       </c>
       <c r="J77" s="2" t="s">
         <v>188</v>
@@ -8685,10 +8702,10 @@
     </row>
     <row r="78" spans="1:10">
       <c r="A78" s="2" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="C78" s="2" t="s">
         <v>419</v>
@@ -8700,10 +8717,10 @@
         <v>6</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="G78" s="12" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="J78" s="2" t="s">
         <v>188</v>
@@ -8711,10 +8728,10 @@
     </row>
     <row r="79" spans="1:10">
       <c r="A79" s="2" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="C79" s="2" t="s">
         <v>419</v>
@@ -8726,7 +8743,7 @@
         <v>6</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>193</v>
+        <v>165</v>
       </c>
       <c r="G79" s="12" t="s">
         <v>405</v>
@@ -8737,10 +8754,10 @@
     </row>
     <row r="80" spans="1:10">
       <c r="A80" s="2" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="C80" s="2" t="s">
         <v>419</v>
@@ -8752,7 +8769,7 @@
         <v>6</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>163</v>
+        <v>193</v>
       </c>
       <c r="G80" s="12" t="s">
         <v>405</v>
@@ -8763,10 +8780,10 @@
     </row>
     <row r="81" spans="1:10">
       <c r="A81" s="2" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="C81" s="2" t="s">
         <v>419</v>
@@ -8778,7 +8795,7 @@
         <v>6</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>197</v>
+        <v>163</v>
       </c>
       <c r="G81" s="12" t="s">
         <v>405</v>
@@ -8789,10 +8806,10 @@
     </row>
     <row r="82" spans="1:10">
       <c r="A82" s="2" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="C82" s="2" t="s">
         <v>419</v>
@@ -8804,7 +8821,7 @@
         <v>6</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="G82" s="12" t="s">
         <v>405</v>
@@ -8815,10 +8832,10 @@
     </row>
     <row r="83" spans="1:10">
       <c r="A83" s="2" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="C83" s="2" t="s">
         <v>419</v>
@@ -8830,24 +8847,21 @@
         <v>6</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="G83" s="12" t="s">
-        <v>347</v>
-      </c>
-      <c r="H83" s="12" t="s">
-        <v>349</v>
+        <v>405</v>
       </c>
       <c r="J83" s="2" t="s">
-        <v>82</v>
+        <v>188</v>
       </c>
     </row>
     <row r="84" spans="1:10">
       <c r="A84" s="2" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="C84" s="2" t="s">
         <v>419</v>
@@ -8859,7 +8873,7 @@
         <v>6</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="G84" s="12" t="s">
         <v>347</v>
@@ -8873,10 +8887,10 @@
     </row>
     <row r="85" spans="1:10">
       <c r="A85" s="2" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>215</v>
+        <v>587</v>
       </c>
       <c r="C85" s="2" t="s">
         <v>419</v>
@@ -8888,7 +8902,7 @@
         <v>6</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="G85" s="12" t="s">
         <v>347</v>
@@ -8902,22 +8916,22 @@
     </row>
     <row r="86" spans="1:10">
       <c r="A86" s="2" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>590</v>
+        <v>215</v>
       </c>
       <c r="C86" s="2" t="s">
         <v>419</v>
       </c>
       <c r="D86" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E86" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>91</v>
+        <v>207</v>
       </c>
       <c r="G86" s="12" t="s">
         <v>347</v>
@@ -8931,22 +8945,22 @@
     </row>
     <row r="87" spans="1:10">
       <c r="A87" s="2" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="C87" s="2" t="s">
         <v>419</v>
       </c>
       <c r="D87" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E87" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="G87" s="12" t="s">
         <v>347</v>
@@ -8960,10 +8974,10 @@
     </row>
     <row r="88" spans="1:10">
       <c r="A88" s="2" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="C88" s="2" t="s">
         <v>419</v>
@@ -8975,7 +8989,7 @@
         <v>6</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>595</v>
+        <v>89</v>
       </c>
       <c r="G88" s="12" t="s">
         <v>347</v>
@@ -8989,10 +9003,10 @@
     </row>
     <row r="89" spans="1:10">
       <c r="A89" s="2" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="C89" s="2" t="s">
         <v>419</v>
@@ -9004,7 +9018,7 @@
         <v>6</v>
       </c>
       <c r="F89" s="2" t="s">
-        <v>207</v>
+        <v>595</v>
       </c>
       <c r="G89" s="12" t="s">
         <v>347</v>
@@ -9018,10 +9032,10 @@
     </row>
     <row r="90" spans="1:10">
       <c r="A90" s="2" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="C90" s="2" t="s">
         <v>419</v>
@@ -9030,13 +9044,16 @@
         <v>3</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>600</v>
-      </c>
-      <c r="G90" s="2" t="s">
-        <v>327</v>
+        <v>207</v>
+      </c>
+      <c r="G90" s="12" t="s">
+        <v>347</v>
+      </c>
+      <c r="H90" s="12" t="s">
+        <v>349</v>
       </c>
       <c r="J90" s="2" t="s">
         <v>82</v>
@@ -9044,36 +9061,36 @@
     </row>
     <row r="91" spans="1:10">
       <c r="A91" s="2" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="C91" s="2" t="s">
         <v>419</v>
       </c>
       <c r="D91" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E91" s="2" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>213</v>
+        <v>600</v>
       </c>
       <c r="G91" s="2" t="s">
         <v>327</v>
       </c>
       <c r="J91" s="2" t="s">
-        <v>215</v>
+        <v>82</v>
       </c>
     </row>
     <row r="92" spans="1:10">
       <c r="A92" s="2" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="C92" s="2" t="s">
         <v>419</v>
@@ -9085,7 +9102,7 @@
         <v>6</v>
       </c>
       <c r="F92" s="2" t="s">
-        <v>91</v>
+        <v>213</v>
       </c>
       <c r="G92" s="2" t="s">
         <v>327</v>
@@ -9096,22 +9113,22 @@
     </row>
     <row r="93" spans="1:10">
       <c r="A93" s="2" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="C93" s="2" t="s">
         <v>419</v>
       </c>
       <c r="D93" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E93" s="2" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>224</v>
+        <v>91</v>
       </c>
       <c r="G93" s="2" t="s">
         <v>327</v>
@@ -9122,22 +9139,22 @@
     </row>
     <row r="94" spans="1:10">
       <c r="A94" s="2" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="C94" s="2" t="s">
         <v>419</v>
       </c>
       <c r="D94" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E94" s="2" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>248</v>
+        <v>224</v>
       </c>
       <c r="G94" s="2" t="s">
         <v>327</v>
@@ -9148,10 +9165,10 @@
     </row>
     <row r="95" spans="1:10">
       <c r="A95" s="2" t="s">
-        <v>476</v>
+        <v>607</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="C95" s="2" t="s">
         <v>419</v>
@@ -9162,6 +9179,9 @@
       <c r="E95" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="F95" s="2" t="s">
+        <v>248</v>
+      </c>
       <c r="G95" s="2" t="s">
         <v>327</v>
       </c>
@@ -9171,54 +9191,45 @@
     </row>
     <row r="96" spans="1:10">
       <c r="A96" s="2" t="s">
-        <v>610</v>
+        <v>476</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="C96" s="2" t="s">
         <v>419</v>
       </c>
       <c r="D96" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E96" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F96" s="2" t="s">
-        <v>228</v>
-      </c>
       <c r="G96" s="2" t="s">
-        <v>317</v>
-      </c>
-      <c r="H96" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="I96" s="2" t="s">
-        <v>307</v>
+        <v>327</v>
       </c>
       <c r="J96" s="2" t="s">
-        <v>230</v>
+        <v>215</v>
       </c>
     </row>
     <row r="97" spans="1:10">
       <c r="A97" s="2" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="C97" s="2" t="s">
         <v>419</v>
       </c>
       <c r="D97" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E97" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F97" s="2" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="G97" s="2" t="s">
         <v>317</v>
@@ -9235,10 +9246,10 @@
     </row>
     <row r="98" spans="1:10">
       <c r="A98" s="2" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="C98" s="2" t="s">
         <v>419</v>
@@ -9247,10 +9258,10 @@
         <v>2</v>
       </c>
       <c r="E98" s="2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="F98" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="G98" s="2" t="s">
         <v>317</v>
@@ -9267,22 +9278,22 @@
     </row>
     <row r="99" spans="1:10">
       <c r="A99" s="2" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>449</v>
+        <v>419</v>
       </c>
       <c r="D99" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E99" s="2" t="s">
         <v>12</v>
       </c>
       <c r="F99" s="2" t="s">
-        <v>618</v>
+        <v>233</v>
       </c>
       <c r="G99" s="2" t="s">
         <v>317</v>
@@ -9299,22 +9310,22 @@
     </row>
     <row r="100" spans="1:10">
       <c r="A100" s="2" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>451</v>
+        <v>617</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>419</v>
+        <v>449</v>
       </c>
       <c r="D100" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E100" s="2" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="F100" s="2" t="s">
-        <v>241</v>
+        <v>618</v>
       </c>
       <c r="G100" s="2" t="s">
         <v>317</v>
@@ -9331,10 +9342,10 @@
     </row>
     <row r="101" spans="1:10">
       <c r="A101" s="2" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>621</v>
+        <v>451</v>
       </c>
       <c r="C101" s="2" t="s">
         <v>419</v>
@@ -9346,21 +9357,27 @@
         <v>6</v>
       </c>
       <c r="F101" s="2" t="s">
-        <v>622</v>
+        <v>241</v>
       </c>
       <c r="G101" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="H101" s="2" t="s">
         <v>296</v>
       </c>
+      <c r="I101" s="2" t="s">
+        <v>307</v>
+      </c>
       <c r="J101" s="2" t="s">
-        <v>245</v>
+        <v>230</v>
       </c>
     </row>
     <row r="102" spans="1:10">
       <c r="A102" s="2" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>624</v>
+        <v>621</v>
       </c>
       <c r="C102" s="2" t="s">
         <v>419</v>
@@ -9372,10 +9389,10 @@
         <v>6</v>
       </c>
       <c r="F102" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="G102" s="12" t="s">
-        <v>303</v>
+        <v>622</v>
+      </c>
+      <c r="G102" s="2" t="s">
+        <v>296</v>
       </c>
       <c r="J102" s="2" t="s">
         <v>245</v>
@@ -9383,10 +9400,10 @@
     </row>
     <row r="103" spans="1:10">
       <c r="A103" s="2" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="C103" s="2" t="s">
         <v>419</v>
@@ -9398,7 +9415,7 @@
         <v>6</v>
       </c>
       <c r="F103" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="G103" s="12" t="s">
         <v>303</v>
@@ -9409,22 +9426,22 @@
     </row>
     <row r="104" spans="1:10">
       <c r="A104" s="2" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="C104" s="2" t="s">
         <v>419</v>
       </c>
       <c r="D104" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E104" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F104" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G104" s="12" t="s">
         <v>303</v>
@@ -9435,22 +9452,22 @@
     </row>
     <row r="105" spans="1:10">
       <c r="A105" s="2" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="C105" s="2" t="s">
         <v>419</v>
       </c>
       <c r="D105" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E105" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F105" s="2" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="G105" s="12" t="s">
         <v>303</v>
@@ -9461,13 +9478,13 @@
     </row>
     <row r="106" spans="1:10">
       <c r="A106" s="2" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>449</v>
+        <v>419</v>
       </c>
       <c r="D106" s="2">
         <v>2</v>
@@ -9476,7 +9493,7 @@
         <v>6</v>
       </c>
       <c r="F106" s="2" t="s">
-        <v>633</v>
+        <v>250</v>
       </c>
       <c r="G106" s="12" t="s">
         <v>303</v>
@@ -9487,13 +9504,13 @@
     </row>
     <row r="107" spans="1:10">
       <c r="A107" s="2" t="s">
-        <v>634</v>
+        <v>631</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>635</v>
+        <v>632</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>419</v>
+        <v>449</v>
       </c>
       <c r="D107" s="2">
         <v>2</v>
@@ -9502,7 +9519,7 @@
         <v>6</v>
       </c>
       <c r="F107" s="2" t="s">
-        <v>228</v>
+        <v>633</v>
       </c>
       <c r="G107" s="12" t="s">
         <v>303</v>
@@ -9513,10 +9530,10 @@
     </row>
     <row r="108" spans="1:10">
       <c r="A108" s="2" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="C108" s="2" t="s">
         <v>419</v>
@@ -9527,6 +9544,9 @@
       <c r="E108" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="F108" s="2" t="s">
+        <v>228</v>
+      </c>
       <c r="G108" s="12" t="s">
         <v>303</v>
       </c>
@@ -9536,22 +9556,22 @@
     </row>
     <row r="109" spans="1:10">
       <c r="A109" s="2" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>449</v>
+        <v>419</v>
       </c>
       <c r="D109" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E109" s="2" t="s">
         <v>6</v>
       </c>
       <c r="G109" s="12" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="J109" s="2" t="s">
         <v>245</v>
@@ -9559,13 +9579,13 @@
     </row>
     <row r="110" spans="1:10">
       <c r="A110" s="2" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>419</v>
+        <v>449</v>
       </c>
       <c r="D110" s="2">
         <v>3</v>
@@ -9573,11 +9593,8 @@
       <c r="E110" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F110" s="2" t="s">
-        <v>254</v>
-      </c>
-      <c r="G110" s="2" t="s">
-        <v>315</v>
+      <c r="G110" s="12" t="s">
+        <v>305</v>
       </c>
       <c r="J110" s="2" t="s">
         <v>245</v>
@@ -9585,36 +9602,36 @@
     </row>
     <row r="111" spans="1:10">
       <c r="A111" s="2" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="C111" s="2" t="s">
         <v>419</v>
       </c>
       <c r="D111" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E111" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F111" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="G111" s="2" t="s">
-        <v>307</v>
+        <v>315</v>
       </c>
       <c r="J111" s="2" t="s">
-        <v>258</v>
+        <v>245</v>
       </c>
     </row>
     <row r="112" spans="1:10">
       <c r="A112" s="2" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="C112" s="2" t="s">
         <v>419</v>
@@ -9628,8 +9645,8 @@
       <c r="F112" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="G112" s="12" t="s">
-        <v>313</v>
+      <c r="G112" s="2" t="s">
+        <v>307</v>
       </c>
       <c r="J112" s="2" t="s">
         <v>258</v>
@@ -9637,10 +9654,10 @@
     </row>
     <row r="113" spans="1:10">
       <c r="A113" s="2" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>635</v>
+        <v>645</v>
       </c>
       <c r="C113" s="2" t="s">
         <v>419</v>
@@ -9652,7 +9669,7 @@
         <v>6</v>
       </c>
       <c r="F113" s="2" t="s">
-        <v>228</v>
+        <v>256</v>
       </c>
       <c r="G113" s="12" t="s">
         <v>313</v>
@@ -9663,10 +9680,10 @@
     </row>
     <row r="114" spans="1:10">
       <c r="A114" s="2" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>648</v>
+        <v>635</v>
       </c>
       <c r="C114" s="2" t="s">
         <v>419</v>
@@ -9678,7 +9695,7 @@
         <v>6</v>
       </c>
       <c r="F114" s="2" t="s">
-        <v>259</v>
+        <v>228</v>
       </c>
       <c r="G114" s="12" t="s">
         <v>313</v>
@@ -9689,22 +9706,25 @@
     </row>
     <row r="115" spans="1:10">
       <c r="A115" s="2" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>449</v>
+        <v>419</v>
       </c>
       <c r="D115" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E115" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="F115" s="2" t="s">
+        <v>259</v>
+      </c>
       <c r="G115" s="12" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="J115" s="2" t="s">
         <v>258</v>
@@ -9712,22 +9732,19 @@
     </row>
     <row r="116" spans="1:10">
       <c r="A116" s="2" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>419</v>
+        <v>449</v>
       </c>
       <c r="D116" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E116" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="F116" s="2" t="s">
-        <v>231</v>
       </c>
       <c r="G116" s="12" t="s">
         <v>315</v>
@@ -9738,22 +9755,22 @@
     </row>
     <row r="117" spans="1:10">
       <c r="A117" s="2" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="C117" s="2" t="s">
         <v>419</v>
       </c>
       <c r="D117" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E117" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F117" s="2" t="s">
-        <v>256</v>
+        <v>231</v>
       </c>
       <c r="G117" s="12" t="s">
         <v>315</v>
@@ -9764,22 +9781,22 @@
     </row>
     <row r="118" spans="1:10">
       <c r="A118" s="2" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="C118" s="2" t="s">
         <v>419</v>
       </c>
       <c r="D118" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E118" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F118" s="2" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="G118" s="12" t="s">
         <v>315</v>
@@ -9790,10 +9807,10 @@
     </row>
     <row r="119" spans="1:10">
       <c r="A119" s="2" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="C119" s="2" t="s">
         <v>419</v>
@@ -9804,6 +9821,9 @@
       <c r="E119" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="F119" s="2" t="s">
+        <v>261</v>
+      </c>
       <c r="G119" s="12" t="s">
         <v>315</v>
       </c>
@@ -9813,36 +9833,33 @@
     </row>
     <row r="120" spans="1:10">
       <c r="A120" s="2" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="C120" s="2" t="s">
         <v>419</v>
       </c>
       <c r="D120" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E120" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F120" s="2" t="s">
-        <v>263</v>
-      </c>
-      <c r="G120" s="2" t="s">
-        <v>666</v>
+      <c r="G120" s="12" t="s">
+        <v>315</v>
       </c>
       <c r="J120" s="2" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
     </row>
     <row r="121" spans="1:10">
       <c r="A121" s="2" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="C121" s="2" t="s">
         <v>419</v>
@@ -9854,7 +9871,7 @@
         <v>6</v>
       </c>
       <c r="F121" s="2" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="G121" s="2" t="s">
         <v>666</v>
@@ -9865,10 +9882,10 @@
     </row>
     <row r="122" spans="1:10">
       <c r="A122" s="2" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="C122" s="2" t="s">
         <v>419</v>
@@ -9880,7 +9897,7 @@
         <v>6</v>
       </c>
       <c r="F122" s="2" t="s">
-        <v>665</v>
+        <v>266</v>
       </c>
       <c r="G122" s="2" t="s">
         <v>666</v>
@@ -9891,10 +9908,10 @@
     </row>
     <row r="123" spans="1:10">
       <c r="A123" s="2" t="s">
-        <v>667</v>
+        <v>663</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>668</v>
+        <v>664</v>
       </c>
       <c r="C123" s="2" t="s">
         <v>419</v>
@@ -9906,7 +9923,7 @@
         <v>6</v>
       </c>
       <c r="F123" s="2" t="s">
-        <v>270</v>
+        <v>665</v>
       </c>
       <c r="G123" s="2" t="s">
         <v>666</v>
@@ -9917,10 +9934,10 @@
     </row>
     <row r="124" spans="1:10">
       <c r="A124" s="2" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="C124" s="2" t="s">
         <v>419</v>
@@ -9931,6 +9948,9 @@
       <c r="E124" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="F124" s="2" t="s">
+        <v>270</v>
+      </c>
       <c r="G124" s="2" t="s">
         <v>666</v>
       </c>
@@ -9940,22 +9960,19 @@
     </row>
     <row r="125" spans="1:10">
       <c r="A125" s="2" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>449</v>
+        <v>419</v>
       </c>
       <c r="D125" s="2">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E125" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="F125" s="2" t="s">
-        <v>263</v>
       </c>
       <c r="G125" s="2" t="s">
         <v>666</v>
@@ -9966,22 +9983,22 @@
     </row>
     <row r="126" spans="1:10">
       <c r="A126" s="2" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>419</v>
+        <v>449</v>
       </c>
       <c r="D126" s="2">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E126" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F126" s="2" t="s">
-        <v>675</v>
+        <v>263</v>
       </c>
       <c r="G126" s="2" t="s">
         <v>666</v>
@@ -9992,10 +10009,10 @@
     </row>
     <row r="127" spans="1:10">
       <c r="A127" s="2" t="s">
-        <v>676</v>
+        <v>673</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>677</v>
+        <v>674</v>
       </c>
       <c r="C127" s="2" t="s">
         <v>419</v>
@@ -10007,7 +10024,7 @@
         <v>6</v>
       </c>
       <c r="F127" s="2" t="s">
-        <v>274</v>
+        <v>675</v>
       </c>
       <c r="G127" s="2" t="s">
         <v>666</v>
@@ -10018,10 +10035,10 @@
     </row>
     <row r="128" spans="1:10">
       <c r="A128" s="2" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="C128" s="2" t="s">
         <v>419</v>
@@ -10033,7 +10050,7 @@
         <v>6</v>
       </c>
       <c r="F128" s="2" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="G128" s="2" t="s">
         <v>666</v>
@@ -10044,10 +10061,10 @@
     </row>
     <row r="129" spans="1:10">
       <c r="A129" s="2" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="C129" s="2" t="s">
         <v>419</v>
@@ -10059,21 +10076,21 @@
         <v>6</v>
       </c>
       <c r="F129" s="2" t="s">
-        <v>595</v>
+        <v>276</v>
       </c>
       <c r="G129" s="2" t="s">
-        <v>682</v>
+        <v>666</v>
       </c>
       <c r="J129" s="2" t="s">
-        <v>280</v>
+        <v>265</v>
       </c>
     </row>
     <row r="130" spans="1:10">
       <c r="A130" s="2" t="s">
-        <v>683</v>
+        <v>680</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>684</v>
+        <v>681</v>
       </c>
       <c r="C130" s="2" t="s">
         <v>419</v>
@@ -10084,6 +10101,9 @@
       <c r="E130" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="F130" s="2" t="s">
+        <v>595</v>
+      </c>
       <c r="G130" s="2" t="s">
         <v>682</v>
       </c>
@@ -10093,10 +10113,10 @@
     </row>
     <row r="131" spans="1:10">
       <c r="A131" s="2" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="C131" s="2" t="s">
         <v>419</v>
@@ -10107,9 +10127,6 @@
       <c r="E131" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F131" s="2" t="s">
-        <v>278</v>
-      </c>
       <c r="G131" s="2" t="s">
         <v>682</v>
       </c>
@@ -10119,10 +10136,10 @@
     </row>
     <row r="132" spans="1:10">
       <c r="A132" s="2" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="C132" s="2" t="s">
         <v>419</v>
@@ -10134,7 +10151,7 @@
         <v>6</v>
       </c>
       <c r="F132" s="2" t="s">
-        <v>211</v>
+        <v>278</v>
       </c>
       <c r="G132" s="2" t="s">
         <v>682</v>
@@ -10145,10 +10162,10 @@
     </row>
     <row r="133" spans="1:10">
       <c r="A133" s="2" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="C133" s="2" t="s">
         <v>419</v>
@@ -10160,7 +10177,7 @@
         <v>6</v>
       </c>
       <c r="F133" s="2" t="s">
-        <v>91</v>
+        <v>211</v>
       </c>
       <c r="G133" s="2" t="s">
         <v>682</v>
@@ -10171,10 +10188,10 @@
     </row>
     <row r="134" spans="1:10">
       <c r="A134" s="2" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="C134" s="2" t="s">
         <v>419</v>
@@ -10186,21 +10203,21 @@
         <v>6</v>
       </c>
       <c r="F134" s="2" t="s">
-        <v>281</v>
-      </c>
-      <c r="G134" s="12" t="s">
-        <v>736</v>
+        <v>91</v>
+      </c>
+      <c r="G134" s="2" t="s">
+        <v>682</v>
       </c>
       <c r="J134" s="2" t="s">
-        <v>160</v>
+        <v>280</v>
       </c>
     </row>
     <row r="135" spans="1:10">
       <c r="A135" s="2" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="C135" s="2" t="s">
         <v>419</v>
@@ -10212,7 +10229,7 @@
         <v>6</v>
       </c>
       <c r="F135" s="2" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="G135" s="12" t="s">
         <v>736</v>
@@ -10223,10 +10240,10 @@
     </row>
     <row r="136" spans="1:10">
       <c r="A136" s="2" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="C136" s="2" t="s">
         <v>419</v>
@@ -10238,7 +10255,7 @@
         <v>6</v>
       </c>
       <c r="F136" s="2" t="s">
-        <v>142</v>
+        <v>283</v>
       </c>
       <c r="G136" s="12" t="s">
         <v>736</v>
@@ -10249,10 +10266,10 @@
     </row>
     <row r="137" spans="1:10">
       <c r="A137" s="2" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="C137" s="2" t="s">
         <v>419</v>
@@ -10264,7 +10281,7 @@
         <v>6</v>
       </c>
       <c r="F137" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G137" s="12" t="s">
         <v>736</v>
@@ -10275,10 +10292,10 @@
     </row>
     <row r="138" spans="1:10">
       <c r="A138" s="2" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
       <c r="C138" s="2" t="s">
         <v>419</v>
@@ -10290,7 +10307,7 @@
         <v>6</v>
       </c>
       <c r="F138" s="2" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="G138" s="12" t="s">
         <v>736</v>
@@ -10301,10 +10318,10 @@
     </row>
     <row r="139" spans="1:10">
       <c r="A139" s="2" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="C139" s="2" t="s">
         <v>419</v>
@@ -10316,7 +10333,7 @@
         <v>6</v>
       </c>
       <c r="F139" s="2" t="s">
-        <v>195</v>
+        <v>152</v>
       </c>
       <c r="G139" s="12" t="s">
         <v>736</v>
@@ -10327,10 +10344,10 @@
     </row>
     <row r="140" spans="1:10">
       <c r="A140" s="2" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
       <c r="C140" s="2" t="s">
         <v>419</v>
@@ -10342,7 +10359,7 @@
         <v>6</v>
       </c>
       <c r="F140" s="2" t="s">
-        <v>281</v>
+        <v>195</v>
       </c>
       <c r="G140" s="12" t="s">
         <v>736</v>
@@ -10353,10 +10370,10 @@
     </row>
     <row r="141" spans="1:10">
       <c r="A141" s="2" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
       <c r="C141" s="2" t="s">
         <v>419</v>
@@ -10368,7 +10385,7 @@
         <v>6</v>
       </c>
       <c r="F141" s="2" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="G141" s="12" t="s">
         <v>736</v>
@@ -10379,10 +10396,10 @@
     </row>
     <row r="142" spans="1:10">
       <c r="A142" s="2" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="C142" s="2" t="s">
         <v>419</v>
@@ -10394,7 +10411,7 @@
         <v>6</v>
       </c>
       <c r="F142" s="2" t="s">
-        <v>709</v>
+        <v>283</v>
       </c>
       <c r="G142" s="12" t="s">
         <v>736</v>
@@ -10405,10 +10422,10 @@
     </row>
     <row r="143" spans="1:10">
       <c r="A143" s="2" t="s">
-        <v>710</v>
+        <v>707</v>
       </c>
       <c r="B143" s="2" t="s">
-        <v>711</v>
+        <v>708</v>
       </c>
       <c r="C143" s="2" t="s">
         <v>419</v>
@@ -10420,7 +10437,7 @@
         <v>6</v>
       </c>
       <c r="F143" s="2" t="s">
-        <v>142</v>
+        <v>709</v>
       </c>
       <c r="G143" s="12" t="s">
         <v>736</v>
@@ -10431,10 +10448,10 @@
     </row>
     <row r="144" spans="1:10">
       <c r="A144" s="2" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="C144" s="2" t="s">
         <v>419</v>
@@ -10445,6 +10462,9 @@
       <c r="E144" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="F144" s="2" t="s">
+        <v>142</v>
+      </c>
       <c r="G144" s="12" t="s">
         <v>736</v>
       </c>
@@ -10454,10 +10474,10 @@
     </row>
     <row r="145" spans="1:10">
       <c r="A145" s="2" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="C145" s="2" t="s">
         <v>419</v>
@@ -10468,9 +10488,6 @@
       <c r="E145" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F145" s="2" t="s">
-        <v>144</v>
-      </c>
       <c r="G145" s="12" t="s">
         <v>736</v>
       </c>
@@ -10480,10 +10497,10 @@
     </row>
     <row r="146" spans="1:10">
       <c r="A146" s="2" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
       <c r="C146" s="2" t="s">
         <v>419</v>
@@ -10495,7 +10512,7 @@
         <v>6</v>
       </c>
       <c r="F146" s="2" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="G146" s="12" t="s">
         <v>736</v>
@@ -10506,10 +10523,10 @@
     </row>
     <row r="147" spans="1:10">
       <c r="A147" s="2" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="C147" s="2" t="s">
         <v>419</v>
@@ -10521,7 +10538,7 @@
         <v>6</v>
       </c>
       <c r="F147" s="2" t="s">
-        <v>195</v>
+        <v>152</v>
       </c>
       <c r="G147" s="12" t="s">
         <v>736</v>
@@ -10532,19 +10549,22 @@
     </row>
     <row r="148" spans="1:10">
       <c r="A148" s="2" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>672</v>
+        <v>719</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>449</v>
+        <v>419</v>
       </c>
       <c r="D148" s="2">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E148" s="2" t="s">
         <v>6</v>
+      </c>
+      <c r="F148" s="2" t="s">
+        <v>195</v>
       </c>
       <c r="G148" s="12" t="s">
         <v>736</v>
@@ -10555,22 +10575,19 @@
     </row>
     <row r="149" spans="1:10">
       <c r="A149" s="2" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>722</v>
+        <v>672</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>419</v>
+        <v>449</v>
       </c>
       <c r="D149" s="2">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E149" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="F149" s="2" t="s">
-        <v>287</v>
       </c>
       <c r="G149" s="12" t="s">
         <v>736</v>
@@ -10579,9 +10596,35 @@
         <v>160</v>
       </c>
     </row>
+    <row r="150" spans="1:10">
+      <c r="A150" s="2" t="s">
+        <v>721</v>
+      </c>
+      <c r="B150" s="2" t="s">
+        <v>722</v>
+      </c>
+      <c r="C150" s="2" t="s">
+        <v>419</v>
+      </c>
+      <c r="D150" s="2">
+        <v>3</v>
+      </c>
+      <c r="E150" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F150" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="G150" s="12" t="s">
+        <v>736</v>
+      </c>
+      <c r="J150" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F45" r:id="rId1"/>
+    <hyperlink ref="F46" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Adjustment to the Available days and times input
</commit_message>
<xml_diff>
--- a/data/Timetable_Input_Template.xlsx
+++ b/data/Timetable_Input_Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jamil\Downloads\PAU_Timetable_Scheduler\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E444C53-F6D5-4BEB-B21A-41FBAD1925E2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1028E916-39CF-4476-A896-C23B3E033402}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11388" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1772" uniqueCount="640">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1772" uniqueCount="648">
   <si>
     <t>Room Name</t>
   </si>
@@ -1946,6 +1946,30 @@
   </si>
   <si>
     <t>14:00-17:00</t>
+  </si>
+  <si>
+    <t>Tue</t>
+  </si>
+  <si>
+    <t>Tue, Wed,Fri</t>
+  </si>
+  <si>
+    <t>Thu</t>
+  </si>
+  <si>
+    <t>Mon,Wed, Thu</t>
+  </si>
+  <si>
+    <t>Tue, Thu</t>
+  </si>
+  <si>
+    <t>Mon,Wed, Fri</t>
+  </si>
+  <si>
+    <t>Mon,Tue</t>
+  </si>
+  <si>
+    <t>Wed,Thu</t>
   </si>
 </sst>
 </file>
@@ -3006,8 +3030,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I111"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G94" sqref="G94"/>
+    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="E97" sqref="E97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -3205,7 +3229,7 @@
         <v>67</v>
       </c>
       <c r="E9" t="s">
-        <v>632</v>
+        <v>641</v>
       </c>
       <c r="F9" s="9" t="s">
         <v>639</v>
@@ -3225,7 +3249,7 @@
         <v>67</v>
       </c>
       <c r="E10" t="s">
-        <v>628</v>
+        <v>642</v>
       </c>
       <c r="F10" s="9" t="s">
         <v>638</v>
@@ -3345,7 +3369,7 @@
         <v>67</v>
       </c>
       <c r="E16" t="s">
-        <v>633</v>
+        <v>643</v>
       </c>
       <c r="F16" s="9" t="s">
         <v>638</v>
@@ -3425,7 +3449,7 @@
         <v>67</v>
       </c>
       <c r="E20" t="s">
-        <v>629</v>
+        <v>644</v>
       </c>
       <c r="F20" s="9" t="s">
         <v>639</v>
@@ -4605,7 +4629,7 @@
         <v>67</v>
       </c>
       <c r="E79" t="s">
-        <v>628</v>
+        <v>640</v>
       </c>
       <c r="F79" s="9" t="s">
         <v>639</v>
@@ -4625,7 +4649,7 @@
         <v>67</v>
       </c>
       <c r="E80" t="s">
-        <v>632</v>
+        <v>647</v>
       </c>
       <c r="F80" s="9" t="s">
         <v>639</v>
@@ -4685,7 +4709,7 @@
         <v>67</v>
       </c>
       <c r="E83" t="s">
-        <v>630</v>
+        <v>646</v>
       </c>
       <c r="F83" s="9" t="s">
         <v>639</v>
@@ -4785,7 +4809,7 @@
         <v>67</v>
       </c>
       <c r="E88" t="s">
-        <v>633</v>
+        <v>645</v>
       </c>
       <c r="F88" s="9" t="s">
         <v>639</v>
@@ -4945,7 +4969,7 @@
         <v>67</v>
       </c>
       <c r="E96" t="s">
-        <v>629</v>
+        <v>640</v>
       </c>
       <c r="F96" s="9" t="s">
         <v>638</v>

</xml_diff>

<commit_message>
Adjusted Impossible Adjunct required hours
</commit_message>
<xml_diff>
--- a/data/Timetable_Input_Template.xlsx
+++ b/data/Timetable_Input_Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jamil\Downloads\PAU_Timetable_Scheduler\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1028E916-39CF-4476-A896-C23B3E033402}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02AFF492-228C-4C98-8E3C-9F87E264C12E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11388" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1772" uniqueCount="648">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1778" uniqueCount="652">
   <si>
     <t>Room Name</t>
   </si>
@@ -1954,22 +1954,34 @@
     <t>Tue, Wed,Fri</t>
   </si>
   <si>
-    <t>Thu</t>
-  </si>
-  <si>
     <t>Mon,Wed, Thu</t>
   </si>
   <si>
-    <t>Tue, Thu</t>
-  </si>
-  <si>
     <t>Mon,Wed, Fri</t>
   </si>
   <si>
-    <t>Mon,Tue</t>
-  </si>
-  <si>
     <t>Wed,Thu</t>
+  </si>
+  <si>
+    <t>Dr E O</t>
+  </si>
+  <si>
+    <t>Mon, Tue, Thu</t>
+  </si>
+  <si>
+    <t>Tue, Wed, Fri</t>
+  </si>
+  <si>
+    <t>Mon, Tue,Wed, Thu</t>
+  </si>
+  <si>
+    <t>Mon, Tue</t>
+  </si>
+  <si>
+    <t>Mon,Tue, Thu</t>
+  </si>
+  <si>
+    <t>Mon, Tue, Wed</t>
   </si>
 </sst>
 </file>
@@ -3028,10 +3040,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I111"/>
+  <dimension ref="A1:I112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="E97" sqref="E97"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -3236,7 +3248,7 @@
       </c>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="12" t="s">
         <v>74</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -3249,7 +3261,7 @@
         <v>67</v>
       </c>
       <c r="E10" t="s">
-        <v>642</v>
+        <v>646</v>
       </c>
       <c r="F10" s="9" t="s">
         <v>638</v>
@@ -3269,7 +3281,7 @@
         <v>67</v>
       </c>
       <c r="E11" t="s">
-        <v>631</v>
+        <v>647</v>
       </c>
       <c r="F11" s="9" t="s">
         <v>639</v>
@@ -3369,7 +3381,7 @@
         <v>67</v>
       </c>
       <c r="E16" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="F16" s="9" t="s">
         <v>638</v>
@@ -3449,7 +3461,7 @@
         <v>67</v>
       </c>
       <c r="E20" t="s">
-        <v>644</v>
+        <v>648</v>
       </c>
       <c r="F20" s="9" t="s">
         <v>639</v>
@@ -3657,10 +3669,10 @@
     </row>
     <row r="31" spans="1:6">
       <c r="A31" s="2" t="s">
-        <v>118</v>
+        <v>465</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>119</v>
+        <v>645</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>120</v>
@@ -3677,10 +3689,10 @@
     </row>
     <row r="32" spans="1:6">
       <c r="A32" s="2" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>120</v>
@@ -3697,10 +3709,10 @@
     </row>
     <row r="33" spans="1:6">
       <c r="A33" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>120</v>
@@ -3717,70 +3729,70 @@
     </row>
     <row r="34" spans="1:6">
       <c r="A34" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>120</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="E34" t="s">
-        <v>633</v>
-      </c>
-      <c r="F34" s="9" t="s">
-        <v>639</v>
+        <v>637</v>
+      </c>
+      <c r="F34" t="s">
+        <v>637</v>
       </c>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>120</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="E35" t="s">
-        <v>637</v>
-      </c>
-      <c r="F35" t="s">
-        <v>637</v>
+        <v>633</v>
+      </c>
+      <c r="F35" s="9" t="s">
+        <v>639</v>
       </c>
     </row>
     <row r="36" spans="1:6">
       <c r="A36" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>120</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="E36" t="s">
-        <v>629</v>
-      </c>
-      <c r="F36" s="9" t="s">
-        <v>639</v>
+        <v>637</v>
+      </c>
+      <c r="F36" t="s">
+        <v>637</v>
       </c>
     </row>
     <row r="37" spans="1:6">
       <c r="A37" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>120</v>
@@ -3789,38 +3801,38 @@
         <v>67</v>
       </c>
       <c r="E37" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="F37" s="9" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
     </row>
     <row r="38" spans="1:6">
       <c r="A38" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="E38" t="s">
-        <v>637</v>
-      </c>
-      <c r="F38" t="s">
-        <v>637</v>
+        <v>631</v>
+      </c>
+      <c r="F38" s="9" t="s">
+        <v>638</v>
       </c>
     </row>
     <row r="39" spans="1:6">
       <c r="A39" s="2" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>135</v>
@@ -3837,10 +3849,10 @@
     </row>
     <row r="40" spans="1:6">
       <c r="A40" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>135</v>
@@ -3857,10 +3869,10 @@
     </row>
     <row r="41" spans="1:6">
       <c r="A41" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>135</v>
@@ -3877,10 +3889,10 @@
     </row>
     <row r="42" spans="1:6">
       <c r="A42" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>135</v>
@@ -3897,30 +3909,30 @@
     </row>
     <row r="43" spans="1:6">
       <c r="A43" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>135</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="E43" t="s">
-        <v>632</v>
-      </c>
-      <c r="F43" s="9" t="s">
-        <v>638</v>
+        <v>637</v>
+      </c>
+      <c r="F43" t="s">
+        <v>637</v>
       </c>
     </row>
     <row r="44" spans="1:6">
       <c r="A44" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>135</v>
@@ -3929,7 +3941,7 @@
         <v>67</v>
       </c>
       <c r="E44" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="F44" s="9" t="s">
         <v>638</v>
@@ -3937,30 +3949,30 @@
     </row>
     <row r="45" spans="1:6">
       <c r="A45" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>135</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="E45" t="s">
-        <v>637</v>
-      </c>
-      <c r="F45" t="s">
-        <v>637</v>
+        <v>631</v>
+      </c>
+      <c r="F45" s="9" t="s">
+        <v>638</v>
       </c>
     </row>
     <row r="46" spans="1:6">
       <c r="A46" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>135</v>
@@ -3977,10 +3989,10 @@
     </row>
     <row r="47" spans="1:6">
       <c r="A47" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>135</v>
@@ -3997,50 +4009,50 @@
     </row>
     <row r="48" spans="1:6">
       <c r="A48" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>135</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="E48" t="s">
-        <v>630</v>
-      </c>
-      <c r="F48" s="9" t="s">
-        <v>639</v>
+        <v>637</v>
+      </c>
+      <c r="F48" t="s">
+        <v>637</v>
       </c>
     </row>
     <row r="49" spans="1:6">
       <c r="A49" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>158</v>
+        <v>135</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="E49" t="s">
-        <v>637</v>
-      </c>
-      <c r="F49" t="s">
-        <v>637</v>
+        <v>630</v>
+      </c>
+      <c r="F49" s="9" t="s">
+        <v>639</v>
       </c>
     </row>
     <row r="50" spans="1:6">
       <c r="A50" s="2" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>158</v>
@@ -4057,10 +4069,10 @@
     </row>
     <row r="51" spans="1:6">
       <c r="A51" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>158</v>
@@ -4077,10 +4089,10 @@
     </row>
     <row r="52" spans="1:6">
       <c r="A52" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>158</v>
@@ -4097,10 +4109,10 @@
     </row>
     <row r="53" spans="1:6">
       <c r="A53" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>158</v>
@@ -4117,50 +4129,50 @@
     </row>
     <row r="54" spans="1:6">
       <c r="A54" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>158</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="E54" t="s">
-        <v>629</v>
-      </c>
-      <c r="F54" s="9" t="s">
-        <v>639</v>
+        <v>637</v>
+      </c>
+      <c r="F54" t="s">
+        <v>637</v>
       </c>
     </row>
     <row r="55" spans="1:6">
       <c r="A55" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>171</v>
+        <v>158</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="E55" t="s">
-        <v>637</v>
-      </c>
-      <c r="F55" t="s">
-        <v>637</v>
+        <v>629</v>
+      </c>
+      <c r="F55" s="9" t="s">
+        <v>639</v>
       </c>
     </row>
     <row r="56" spans="1:6">
       <c r="A56" s="2" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>171</v>
@@ -4177,10 +4189,10 @@
     </row>
     <row r="57" spans="1:6">
       <c r="A57" s="2" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>171</v>
@@ -4197,93 +4209,93 @@
     </row>
     <row r="58" spans="1:6">
       <c r="A58" s="2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>171</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="E58" t="s">
-        <v>631</v>
-      </c>
-      <c r="F58" s="9" t="s">
-        <v>639</v>
+        <v>637</v>
+      </c>
+      <c r="F58" t="s">
+        <v>637</v>
       </c>
     </row>
     <row r="59" spans="1:6">
       <c r="A59" s="2" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C59" s="2" t="s">
         <v>171</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="E59" t="s">
-        <v>637</v>
-      </c>
-      <c r="F59" t="s">
-        <v>637</v>
+        <v>631</v>
+      </c>
+      <c r="F59" s="9" t="s">
+        <v>639</v>
       </c>
     </row>
     <row r="60" spans="1:6">
       <c r="A60" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C60" s="2" t="s">
         <v>171</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="E60" t="s">
-        <v>629</v>
-      </c>
-      <c r="F60" s="9" t="s">
-        <v>638</v>
+        <v>637</v>
+      </c>
+      <c r="F60" t="s">
+        <v>637</v>
       </c>
     </row>
     <row r="61" spans="1:6">
       <c r="A61" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>171</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="E61" t="s">
-        <v>637</v>
-      </c>
-      <c r="F61" t="s">
-        <v>637</v>
+        <v>629</v>
+      </c>
+      <c r="F61" s="9" t="s">
+        <v>638</v>
       </c>
     </row>
     <row r="62" spans="1:6">
       <c r="A62" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>186</v>
+        <v>171</v>
       </c>
       <c r="D62" s="2" t="s">
         <v>57</v>
@@ -4297,50 +4309,50 @@
     </row>
     <row r="63" spans="1:6">
       <c r="A63" s="2" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C63" s="2" t="s">
         <v>186</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="E63" t="s">
-        <v>631</v>
-      </c>
-      <c r="F63" s="9" t="s">
-        <v>639</v>
+        <v>637</v>
+      </c>
+      <c r="F63" t="s">
+        <v>637</v>
       </c>
     </row>
     <row r="64" spans="1:6">
       <c r="A64" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C64" s="2" t="s">
         <v>186</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="E64" t="s">
-        <v>637</v>
-      </c>
-      <c r="F64" t="s">
-        <v>637</v>
+        <v>631</v>
+      </c>
+      <c r="F64" s="9" t="s">
+        <v>639</v>
       </c>
     </row>
     <row r="65" spans="1:6">
       <c r="A65" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C65" s="2" t="s">
         <v>186</v>
@@ -4357,10 +4369,10 @@
     </row>
     <row r="66" spans="1:6">
       <c r="A66" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C66" s="2" t="s">
         <v>186</v>
@@ -4377,10 +4389,10 @@
     </row>
     <row r="67" spans="1:6">
       <c r="A67" s="2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C67" s="2" t="s">
         <v>186</v>
@@ -4397,10 +4409,10 @@
     </row>
     <row r="68" spans="1:6">
       <c r="A68" s="2" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C68" s="2" t="s">
         <v>186</v>
@@ -4417,13 +4429,13 @@
     </row>
     <row r="69" spans="1:6">
       <c r="A69" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>82</v>
+        <v>186</v>
       </c>
       <c r="D69" s="2" t="s">
         <v>57</v>
@@ -4437,50 +4449,50 @@
     </row>
     <row r="70" spans="1:6">
       <c r="A70" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C70" s="2" t="s">
         <v>82</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="E70" t="s">
-        <v>628</v>
-      </c>
-      <c r="F70" s="9" t="s">
-        <v>639</v>
+        <v>637</v>
+      </c>
+      <c r="F70" t="s">
+        <v>637</v>
       </c>
     </row>
     <row r="71" spans="1:6">
       <c r="A71" s="2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C71" s="2" t="s">
         <v>82</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="E71" t="s">
-        <v>637</v>
-      </c>
-      <c r="F71" t="s">
-        <v>637</v>
+        <v>649</v>
+      </c>
+      <c r="F71" s="9" t="s">
+        <v>639</v>
       </c>
     </row>
     <row r="72" spans="1:6">
       <c r="A72" s="2" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C72" s="2" t="s">
         <v>82</v>
@@ -4497,10 +4509,10 @@
     </row>
     <row r="73" spans="1:6">
       <c r="A73" s="2" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C73" s="2" t="s">
         <v>82</v>
@@ -4517,10 +4529,10 @@
     </row>
     <row r="74" spans="1:6">
       <c r="A74" s="2" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C74" s="2" t="s">
         <v>82</v>
@@ -4537,13 +4549,13 @@
     </row>
     <row r="75" spans="1:6">
       <c r="A75" s="2" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>213</v>
+        <v>82</v>
       </c>
       <c r="D75" s="2" t="s">
         <v>57</v>
@@ -4557,10 +4569,10 @@
     </row>
     <row r="76" spans="1:6">
       <c r="A76" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="C76" s="2" t="s">
         <v>213</v>
@@ -4577,10 +4589,10 @@
     </row>
     <row r="77" spans="1:6">
       <c r="A77" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C77" s="2" t="s">
         <v>213</v>
@@ -4597,10 +4609,10 @@
     </row>
     <row r="78" spans="1:6">
       <c r="A78" s="2" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C78" s="2" t="s">
         <v>213</v>
@@ -4617,30 +4629,30 @@
     </row>
     <row r="79" spans="1:6">
       <c r="A79" s="2" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C79" s="2" t="s">
         <v>213</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="E79" t="s">
-        <v>640</v>
-      </c>
-      <c r="F79" s="9" t="s">
-        <v>639</v>
+        <v>637</v>
+      </c>
+      <c r="F79" t="s">
+        <v>637</v>
       </c>
     </row>
     <row r="80" spans="1:6">
       <c r="A80" s="2" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C80" s="2" t="s">
         <v>213</v>
@@ -4649,7 +4661,7 @@
         <v>67</v>
       </c>
       <c r="E80" t="s">
-        <v>647</v>
+        <v>640</v>
       </c>
       <c r="F80" s="9" t="s">
         <v>639</v>
@@ -4657,33 +4669,33 @@
     </row>
     <row r="81" spans="1:6">
       <c r="A81" s="2" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C81" s="2" t="s">
         <v>213</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="E81" t="s">
-        <v>637</v>
-      </c>
-      <c r="F81" t="s">
-        <v>637</v>
+        <v>644</v>
+      </c>
+      <c r="F81" s="9" t="s">
+        <v>639</v>
       </c>
     </row>
     <row r="82" spans="1:6">
       <c r="A82" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>228</v>
+        <v>213</v>
       </c>
       <c r="D82" s="2" t="s">
         <v>57</v>
@@ -4697,50 +4709,50 @@
     </row>
     <row r="83" spans="1:6">
       <c r="A83" s="2" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C83" s="2" t="s">
         <v>228</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="E83" t="s">
-        <v>646</v>
-      </c>
-      <c r="F83" s="9" t="s">
-        <v>639</v>
+        <v>637</v>
+      </c>
+      <c r="F83" t="s">
+        <v>637</v>
       </c>
     </row>
     <row r="84" spans="1:6">
       <c r="A84" s="2" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C84" s="2" t="s">
         <v>228</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="E84" t="s">
-        <v>637</v>
-      </c>
-      <c r="F84" t="s">
-        <v>637</v>
+        <v>650</v>
+      </c>
+      <c r="F84" s="9" t="s">
+        <v>639</v>
       </c>
     </row>
     <row r="85" spans="1:6">
       <c r="A85" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C85" s="2" t="s">
         <v>228</v>
@@ -4757,10 +4769,10 @@
     </row>
     <row r="86" spans="1:6">
       <c r="A86" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C86" s="2" t="s">
         <v>228</v>
@@ -4777,10 +4789,10 @@
     </row>
     <row r="87" spans="1:6">
       <c r="A87" s="2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C87" s="2" t="s">
         <v>228</v>
@@ -4797,50 +4809,50 @@
     </row>
     <row r="88" spans="1:6">
       <c r="A88" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C88" s="2" t="s">
         <v>228</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="E88" t="s">
-        <v>645</v>
-      </c>
-      <c r="F88" s="9" t="s">
-        <v>639</v>
+        <v>637</v>
+      </c>
+      <c r="F88" t="s">
+        <v>637</v>
       </c>
     </row>
     <row r="89" spans="1:6">
       <c r="A89" s="2" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>243</v>
+        <v>228</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="E89" t="s">
-        <v>637</v>
-      </c>
-      <c r="F89" t="s">
-        <v>637</v>
+        <v>643</v>
+      </c>
+      <c r="F89" s="9" t="s">
+        <v>639</v>
       </c>
     </row>
     <row r="90" spans="1:6">
       <c r="A90" s="2" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="C90" s="2" t="s">
         <v>243</v>
@@ -4857,10 +4869,10 @@
     </row>
     <row r="91" spans="1:6">
       <c r="A91" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C91" s="2" t="s">
         <v>243</v>
@@ -4877,10 +4889,10 @@
     </row>
     <row r="92" spans="1:6">
       <c r="A92" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C92" s="2" t="s">
         <v>243</v>
@@ -4897,10 +4909,10 @@
     </row>
     <row r="93" spans="1:6">
       <c r="A93" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C93" s="2" t="s">
         <v>243</v>
@@ -4917,10 +4929,10 @@
     </row>
     <row r="94" spans="1:6">
       <c r="A94" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C94" s="2" t="s">
         <v>243</v>
@@ -4937,30 +4949,30 @@
     </row>
     <row r="95" spans="1:6">
       <c r="A95" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>256</v>
+        <v>243</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="E95" t="s">
-        <v>628</v>
-      </c>
-      <c r="F95" s="9" t="s">
-        <v>639</v>
+        <v>637</v>
+      </c>
+      <c r="F95" t="s">
+        <v>637</v>
       </c>
     </row>
     <row r="96" spans="1:6">
       <c r="A96" s="2" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C96" s="2" t="s">
         <v>256</v>
@@ -4969,34 +4981,51 @@
         <v>67</v>
       </c>
       <c r="E96" t="s">
-        <v>640</v>
+        <v>651</v>
       </c>
       <c r="F96" s="9" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
     </row>
     <row r="97" spans="1:6">
       <c r="A97" s="2" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C97" s="2" t="s">
         <v>256</v>
       </c>
       <c r="D97" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E97" t="s">
+        <v>640</v>
+      </c>
+      <c r="F97" s="9" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6">
+      <c r="A98" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="D98" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E97" t="s">
-        <v>637</v>
-      </c>
-      <c r="F97" t="s">
-        <v>637</v>
-      </c>
-    </row>
-    <row r="98" spans="1:6">
-      <c r="F98" s="9"/>
+      <c r="E98" t="s">
+        <v>637</v>
+      </c>
+      <c r="F98" t="s">
+        <v>637</v>
+      </c>
     </row>
     <row r="99" spans="1:6">
       <c r="F99" s="9"/>
@@ -5037,7 +5066,13 @@
     <row r="111" spans="1:6">
       <c r="F111" s="9"/>
     </row>
+    <row r="112" spans="1:6">
+      <c r="F112" s="9"/>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A10" r:id="rId1" xr:uid="{BA3F7FB2-1A63-44AB-9E7D-5DC5328EE8FA}"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -5046,7 +5081,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E56"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
+    <sheetView topLeftCell="A35" workbookViewId="0">
       <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
@@ -6028,8 +6063,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:K150"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D156" sqref="D156"/>
+    <sheetView topLeftCell="A23" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -7212,7 +7247,7 @@
       <c r="E40" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F40" s="2" t="s">
+      <c r="F40" s="12" t="s">
         <v>465</v>
       </c>
       <c r="G40" s="2" t="s">
@@ -9407,6 +9442,7 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F46" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="F40" r:id="rId2" xr:uid="{EACDD31E-E9D9-4E66-823C-5DDB3FEC7E82}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
All known bugs fixed
</commit_message>
<xml_diff>
--- a/data/Timetable_Input_Template.xlsx
+++ b/data/Timetable_Input_Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jamil\Downloads\Timetable scheduler hoster\PAU_Timetable_Scheduler\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16AD6A0F-5E7D-44CB-9FD6-2A5AD83A0457}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9953F2C4-6E20-4E2D-AD75-4EA6060E31CF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11388" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1778" uniqueCount="653">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1772" uniqueCount="653">
   <si>
     <t>Room Name</t>
   </si>
@@ -6066,8 +6066,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:K150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B54" sqref="B54"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G51" sqref="G51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -6302,9 +6302,7 @@
       <c r="H7" s="11" t="s">
         <v>368</v>
       </c>
-      <c r="I7" s="11" t="s">
-        <v>351</v>
-      </c>
+      <c r="I7" s="11"/>
       <c r="J7" s="2" t="s">
         <v>56</v>
       </c>
@@ -6334,9 +6332,7 @@
       <c r="H8" s="11" t="s">
         <v>368</v>
       </c>
-      <c r="I8" s="11" t="s">
-        <v>351</v>
-      </c>
+      <c r="I8" s="11"/>
       <c r="J8" s="2" t="s">
         <v>56</v>
       </c>
@@ -6366,9 +6362,7 @@
       <c r="H9" s="11" t="s">
         <v>368</v>
       </c>
-      <c r="I9" s="11" t="s">
-        <v>351</v>
-      </c>
+      <c r="I9" s="11"/>
       <c r="J9" s="2" t="s">
         <v>56</v>
       </c>
@@ -6398,9 +6392,7 @@
       <c r="H10" s="11" t="s">
         <v>368</v>
       </c>
-      <c r="I10" s="11" t="s">
-        <v>351</v>
-      </c>
+      <c r="I10" s="11"/>
       <c r="J10" s="2" t="s">
         <v>56</v>
       </c>
@@ -6430,9 +6422,7 @@
       <c r="H11" s="11" t="s">
         <v>368</v>
       </c>
-      <c r="I11" s="11" t="s">
-        <v>351</v>
-      </c>
+      <c r="I11" s="11"/>
       <c r="J11" s="2" t="s">
         <v>56</v>
       </c>
@@ -6462,9 +6452,7 @@
       <c r="H12" s="11" t="s">
         <v>368</v>
       </c>
-      <c r="I12" s="11" t="s">
-        <v>351</v>
-      </c>
+      <c r="I12" s="11"/>
       <c r="J12" s="2" t="s">
         <v>56</v>
       </c>

</xml_diff>

<commit_message>
Added Updating Errors when Swapping/Changing Classes
</commit_message>
<xml_diff>
--- a/data/Timetable_Input_Template.xlsx
+++ b/data/Timetable_Input_Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jamil\Downloads\Timetable scheduler hoster\PAU_Timetable_Scheduler\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9953F2C4-6E20-4E2D-AD75-4EA6060E31CF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D077B899-313E-478A-94C3-B269DFA2A48F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11388" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1772" uniqueCount="653">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1759" uniqueCount="649">
   <si>
     <t>Room Name</t>
   </si>
@@ -958,12 +958,6 @@
     <t>Computer Science - Year  2/Stream 1</t>
   </si>
   <si>
-    <t>CSC 200 - 2</t>
-  </si>
-  <si>
-    <t>Computer Science - Year  2/Stream 2</t>
-  </si>
-  <si>
     <t>CSC 300 - 1</t>
   </si>
   <si>
@@ -980,12 +974,6 @@
   </si>
   <si>
     <t>Computer Science - Year  4/Stream 1</t>
-  </si>
-  <si>
-    <t>CSC 400 - 2</t>
-  </si>
-  <si>
-    <t>Computer Science - Year  4/Stream 2</t>
   </si>
   <si>
     <t>ECO 100</t>
@@ -3063,10 +3051,10 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="10" t="s">
-        <v>634</v>
+        <v>630</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>635</v>
+        <v>631</v>
       </c>
       <c r="C1" s="10" t="s">
         <v>50</v>
@@ -3098,10 +3086,10 @@
         <v>57</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="G2" s="8"/>
       <c r="H2" s="8"/>
@@ -3121,10 +3109,10 @@
         <v>57</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="G3" s="8"/>
       <c r="H3" s="8"/>
@@ -3144,10 +3132,10 @@
         <v>57</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -3164,10 +3152,10 @@
         <v>57</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -3187,7 +3175,7 @@
         <v>58</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -3204,10 +3192,10 @@
         <v>57</v>
       </c>
       <c r="E7" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="F7" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -3224,10 +3212,10 @@
         <v>67</v>
       </c>
       <c r="E8" t="s">
-        <v>628</v>
+        <v>624</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>639</v>
+        <v>635</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -3244,10 +3232,10 @@
         <v>67</v>
       </c>
       <c r="E9" t="s">
-        <v>641</v>
+        <v>637</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>639</v>
+        <v>635</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -3264,10 +3252,10 @@
         <v>67</v>
       </c>
       <c r="E10" t="s">
-        <v>646</v>
+        <v>642</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -3284,10 +3272,10 @@
         <v>67</v>
       </c>
       <c r="E11" t="s">
-        <v>647</v>
+        <v>643</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>639</v>
+        <v>635</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -3304,10 +3292,10 @@
         <v>57</v>
       </c>
       <c r="E12" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="F12" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -3324,10 +3312,10 @@
         <v>57</v>
       </c>
       <c r="E13" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="F13" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -3344,10 +3332,10 @@
         <v>57</v>
       </c>
       <c r="E14" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="F14" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -3364,10 +3352,10 @@
         <v>57</v>
       </c>
       <c r="E15" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="F15" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -3384,10 +3372,10 @@
         <v>67</v>
       </c>
       <c r="E16" t="s">
-        <v>642</v>
+        <v>638</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -3404,10 +3392,10 @@
         <v>57</v>
       </c>
       <c r="E17" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="F17" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -3424,10 +3412,10 @@
         <v>57</v>
       </c>
       <c r="E18" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="F18" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -3444,10 +3432,10 @@
         <v>57</v>
       </c>
       <c r="E19" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="F19" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -3464,10 +3452,10 @@
         <v>67</v>
       </c>
       <c r="E20" t="s">
-        <v>648</v>
+        <v>644</v>
       </c>
       <c r="F20" s="9" t="s">
-        <v>639</v>
+        <v>635</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -3484,10 +3472,10 @@
         <v>57</v>
       </c>
       <c r="E21" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="F21" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -3504,10 +3492,10 @@
         <v>57</v>
       </c>
       <c r="E22" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="F22" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -3524,10 +3512,10 @@
         <v>57</v>
       </c>
       <c r="E23" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="F23" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -3544,10 +3532,10 @@
         <v>57</v>
       </c>
       <c r="E24" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="F24" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -3564,10 +3552,10 @@
         <v>57</v>
       </c>
       <c r="E25" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="F25" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -3584,10 +3572,10 @@
         <v>57</v>
       </c>
       <c r="E26" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="F26" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -3604,10 +3592,10 @@
         <v>57</v>
       </c>
       <c r="E27" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="F27" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -3624,10 +3612,10 @@
         <v>67</v>
       </c>
       <c r="E28" t="s">
-        <v>632</v>
+        <v>628</v>
       </c>
       <c r="F28" s="9" t="s">
-        <v>639</v>
+        <v>635</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -3644,10 +3632,10 @@
         <v>57</v>
       </c>
       <c r="E29" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="F29" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -3664,18 +3652,18 @@
         <v>57</v>
       </c>
       <c r="E30" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="F30" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" s="2" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>645</v>
+        <v>641</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>120</v>
@@ -3684,10 +3672,10 @@
         <v>57</v>
       </c>
       <c r="E31" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="F31" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -3704,10 +3692,10 @@
         <v>57</v>
       </c>
       <c r="E32" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="F32" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -3724,10 +3712,10 @@
         <v>57</v>
       </c>
       <c r="E33" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="F33" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -3744,10 +3732,10 @@
         <v>57</v>
       </c>
       <c r="E34" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="F34" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -3764,10 +3752,10 @@
         <v>67</v>
       </c>
       <c r="E35" t="s">
-        <v>633</v>
+        <v>629</v>
       </c>
       <c r="F35" s="9" t="s">
-        <v>639</v>
+        <v>635</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -3784,10 +3772,10 @@
         <v>57</v>
       </c>
       <c r="E36" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="F36" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -3804,10 +3792,10 @@
         <v>67</v>
       </c>
       <c r="E37" t="s">
-        <v>629</v>
+        <v>625</v>
       </c>
       <c r="F37" s="9" t="s">
-        <v>639</v>
+        <v>635</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -3824,10 +3812,10 @@
         <v>67</v>
       </c>
       <c r="E38" t="s">
-        <v>631</v>
+        <v>627</v>
       </c>
       <c r="F38" s="9" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -3844,10 +3832,10 @@
         <v>57</v>
       </c>
       <c r="E39" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="F39" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -3864,10 +3852,10 @@
         <v>57</v>
       </c>
       <c r="E40" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="F40" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -3884,10 +3872,10 @@
         <v>57</v>
       </c>
       <c r="E41" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="F41" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -3904,10 +3892,10 @@
         <v>57</v>
       </c>
       <c r="E42" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="F42" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -3924,10 +3912,10 @@
         <v>57</v>
       </c>
       <c r="E43" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="F43" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -3944,10 +3932,10 @@
         <v>67</v>
       </c>
       <c r="E44" t="s">
-        <v>632</v>
+        <v>628</v>
       </c>
       <c r="F44" s="9" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -3964,10 +3952,10 @@
         <v>67</v>
       </c>
       <c r="E45" t="s">
-        <v>631</v>
+        <v>627</v>
       </c>
       <c r="F45" s="9" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -3984,10 +3972,10 @@
         <v>57</v>
       </c>
       <c r="E46" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="F46" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -4004,10 +3992,10 @@
         <v>57</v>
       </c>
       <c r="E47" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="F47" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -4024,10 +4012,10 @@
         <v>57</v>
       </c>
       <c r="E48" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="F48" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -4044,10 +4032,10 @@
         <v>67</v>
       </c>
       <c r="E49" t="s">
-        <v>630</v>
+        <v>626</v>
       </c>
       <c r="F49" s="9" t="s">
-        <v>639</v>
+        <v>635</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -4064,10 +4052,10 @@
         <v>57</v>
       </c>
       <c r="E50" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="F50" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -4084,10 +4072,10 @@
         <v>57</v>
       </c>
       <c r="E51" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="F51" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
     </row>
     <row r="52" spans="1:6">
@@ -4104,10 +4092,10 @@
         <v>57</v>
       </c>
       <c r="E52" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="F52" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -4124,10 +4112,10 @@
         <v>57</v>
       </c>
       <c r="E53" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="F53" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -4144,10 +4132,10 @@
         <v>57</v>
       </c>
       <c r="E54" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="F54" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -4164,10 +4152,10 @@
         <v>67</v>
       </c>
       <c r="E55" t="s">
-        <v>629</v>
+        <v>625</v>
       </c>
       <c r="F55" s="9" t="s">
-        <v>639</v>
+        <v>635</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -4184,10 +4172,10 @@
         <v>57</v>
       </c>
       <c r="E56" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="F56" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -4204,10 +4192,10 @@
         <v>57</v>
       </c>
       <c r="E57" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="F57" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -4224,10 +4212,10 @@
         <v>57</v>
       </c>
       <c r="E58" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="F58" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -4244,10 +4232,10 @@
         <v>67</v>
       </c>
       <c r="E59" t="s">
-        <v>631</v>
+        <v>627</v>
       </c>
       <c r="F59" s="9" t="s">
-        <v>639</v>
+        <v>635</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -4264,10 +4252,10 @@
         <v>57</v>
       </c>
       <c r="E60" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="F60" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -4284,10 +4272,10 @@
         <v>67</v>
       </c>
       <c r="E61" t="s">
-        <v>629</v>
+        <v>625</v>
       </c>
       <c r="F61" s="9" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -4304,10 +4292,10 @@
         <v>57</v>
       </c>
       <c r="E62" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="F62" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
     </row>
     <row r="63" spans="1:6">
@@ -4324,10 +4312,10 @@
         <v>57</v>
       </c>
       <c r="E63" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="F63" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
     </row>
     <row r="64" spans="1:6">
@@ -4344,10 +4332,10 @@
         <v>67</v>
       </c>
       <c r="E64" t="s">
-        <v>631</v>
+        <v>627</v>
       </c>
       <c r="F64" s="9" t="s">
-        <v>639</v>
+        <v>635</v>
       </c>
     </row>
     <row r="65" spans="1:6">
@@ -4364,10 +4352,10 @@
         <v>57</v>
       </c>
       <c r="E65" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="F65" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
     </row>
     <row r="66" spans="1:6">
@@ -4384,10 +4372,10 @@
         <v>57</v>
       </c>
       <c r="E66" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="F66" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
     </row>
     <row r="67" spans="1:6">
@@ -4404,10 +4392,10 @@
         <v>57</v>
       </c>
       <c r="E67" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="F67" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
     </row>
     <row r="68" spans="1:6">
@@ -4424,10 +4412,10 @@
         <v>57</v>
       </c>
       <c r="E68" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="F68" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
     </row>
     <row r="69" spans="1:6">
@@ -4444,10 +4432,10 @@
         <v>57</v>
       </c>
       <c r="E69" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="F69" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
     </row>
     <row r="70" spans="1:6">
@@ -4464,10 +4452,10 @@
         <v>57</v>
       </c>
       <c r="E70" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="F70" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
     </row>
     <row r="71" spans="1:6">
@@ -4484,10 +4472,10 @@
         <v>67</v>
       </c>
       <c r="E71" t="s">
-        <v>649</v>
+        <v>645</v>
       </c>
       <c r="F71" s="9" t="s">
-        <v>639</v>
+        <v>635</v>
       </c>
     </row>
     <row r="72" spans="1:6">
@@ -4504,10 +4492,10 @@
         <v>57</v>
       </c>
       <c r="E72" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="F72" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
     </row>
     <row r="73" spans="1:6">
@@ -4524,10 +4512,10 @@
         <v>57</v>
       </c>
       <c r="E73" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="F73" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
     </row>
     <row r="74" spans="1:6">
@@ -4544,10 +4532,10 @@
         <v>57</v>
       </c>
       <c r="E74" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="F74" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
     </row>
     <row r="75" spans="1:6">
@@ -4564,10 +4552,10 @@
         <v>57</v>
       </c>
       <c r="E75" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="F75" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
     </row>
     <row r="76" spans="1:6">
@@ -4584,10 +4572,10 @@
         <v>57</v>
       </c>
       <c r="E76" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="F76" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
     </row>
     <row r="77" spans="1:6">
@@ -4604,10 +4592,10 @@
         <v>57</v>
       </c>
       <c r="E77" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="F77" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
     </row>
     <row r="78" spans="1:6">
@@ -4624,10 +4612,10 @@
         <v>57</v>
       </c>
       <c r="E78" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="F78" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
     </row>
     <row r="79" spans="1:6">
@@ -4644,10 +4632,10 @@
         <v>57</v>
       </c>
       <c r="E79" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="F79" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
     </row>
     <row r="80" spans="1:6">
@@ -4664,10 +4652,10 @@
         <v>67</v>
       </c>
       <c r="E80" t="s">
-        <v>640</v>
+        <v>636</v>
       </c>
       <c r="F80" s="9" t="s">
-        <v>639</v>
+        <v>635</v>
       </c>
     </row>
     <row r="81" spans="1:6">
@@ -4684,10 +4672,10 @@
         <v>67</v>
       </c>
       <c r="E81" t="s">
-        <v>644</v>
+        <v>640</v>
       </c>
       <c r="F81" s="9" t="s">
-        <v>639</v>
+        <v>635</v>
       </c>
     </row>
     <row r="82" spans="1:6">
@@ -4704,10 +4692,10 @@
         <v>57</v>
       </c>
       <c r="E82" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="F82" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
     </row>
     <row r="83" spans="1:6">
@@ -4724,10 +4712,10 @@
         <v>57</v>
       </c>
       <c r="E83" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="F83" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
     </row>
     <row r="84" spans="1:6">
@@ -4744,10 +4732,10 @@
         <v>67</v>
       </c>
       <c r="E84" t="s">
-        <v>650</v>
+        <v>646</v>
       </c>
       <c r="F84" s="9" t="s">
-        <v>639</v>
+        <v>635</v>
       </c>
     </row>
     <row r="85" spans="1:6">
@@ -4764,10 +4752,10 @@
         <v>57</v>
       </c>
       <c r="E85" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="F85" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
     </row>
     <row r="86" spans="1:6">
@@ -4784,10 +4772,10 @@
         <v>57</v>
       </c>
       <c r="E86" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="F86" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
     </row>
     <row r="87" spans="1:6">
@@ -4804,10 +4792,10 @@
         <v>57</v>
       </c>
       <c r="E87" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="F87" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
     </row>
     <row r="88" spans="1:6">
@@ -4824,10 +4812,10 @@
         <v>57</v>
       </c>
       <c r="E88" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="F88" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
     </row>
     <row r="89" spans="1:6">
@@ -4844,10 +4832,10 @@
         <v>67</v>
       </c>
       <c r="E89" t="s">
-        <v>643</v>
+        <v>639</v>
       </c>
       <c r="F89" s="9" t="s">
-        <v>639</v>
+        <v>635</v>
       </c>
     </row>
     <row r="90" spans="1:6">
@@ -4864,10 +4852,10 @@
         <v>57</v>
       </c>
       <c r="E90" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="F90" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
     </row>
     <row r="91" spans="1:6">
@@ -4884,10 +4872,10 @@
         <v>57</v>
       </c>
       <c r="E91" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="F91" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
     </row>
     <row r="92" spans="1:6">
@@ -4904,10 +4892,10 @@
         <v>57</v>
       </c>
       <c r="E92" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="F92" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
     </row>
     <row r="93" spans="1:6">
@@ -4924,10 +4912,10 @@
         <v>57</v>
       </c>
       <c r="E93" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="F93" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
     </row>
     <row r="94" spans="1:6">
@@ -4944,10 +4932,10 @@
         <v>57</v>
       </c>
       <c r="E94" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="F94" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
     </row>
     <row r="95" spans="1:6">
@@ -4964,10 +4952,10 @@
         <v>57</v>
       </c>
       <c r="E95" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="F95" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
     </row>
     <row r="96" spans="1:6">
@@ -4984,10 +4972,10 @@
         <v>67</v>
       </c>
       <c r="E96" t="s">
-        <v>651</v>
+        <v>647</v>
       </c>
       <c r="F96" s="9" t="s">
-        <v>639</v>
+        <v>635</v>
       </c>
     </row>
     <row r="97" spans="1:6">
@@ -5004,10 +4992,10 @@
         <v>67</v>
       </c>
       <c r="E97" t="s">
-        <v>640</v>
+        <v>636</v>
       </c>
       <c r="F97" s="9" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
     </row>
     <row r="98" spans="1:6">
@@ -5024,10 +5012,10 @@
         <v>57</v>
       </c>
       <c r="E98" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="F98" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
     </row>
     <row r="99" spans="1:6">
@@ -5082,10 +5070,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:E56"/>
+  <dimension ref="A1:E54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24:XFD24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -5496,13 +5484,13 @@
         <v>311</v>
       </c>
       <c r="C24">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="D24" t="s">
         <v>82</v>
       </c>
       <c r="E24">
-        <v>30</v>
+        <v>35</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -5519,7 +5507,7 @@
         <v>82</v>
       </c>
       <c r="E25">
-        <v>35</v>
+        <v>20</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -5530,13 +5518,13 @@
         <v>315</v>
       </c>
       <c r="C26">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="D26" t="s">
         <v>82</v>
       </c>
       <c r="E26">
-        <v>20</v>
+        <v>30</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -5547,13 +5535,13 @@
         <v>317</v>
       </c>
       <c r="C27">
-        <v>400</v>
+        <v>100</v>
       </c>
       <c r="D27" t="s">
-        <v>82</v>
+        <v>158</v>
       </c>
       <c r="E27">
-        <v>30</v>
+        <v>35</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -5564,13 +5552,13 @@
         <v>319</v>
       </c>
       <c r="C28">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="D28" t="s">
-        <v>82</v>
+        <v>158</v>
       </c>
       <c r="E28">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -5581,13 +5569,13 @@
         <v>321</v>
       </c>
       <c r="C29">
-        <v>100</v>
+        <v>300</v>
       </c>
       <c r="D29" t="s">
         <v>158</v>
       </c>
       <c r="E29">
-        <v>35</v>
+        <v>20</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -5598,13 +5586,13 @@
         <v>323</v>
       </c>
       <c r="C30">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="D30" t="s">
         <v>158</v>
       </c>
       <c r="E30">
-        <v>40</v>
+        <v>25</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -5615,10 +5603,10 @@
         <v>325</v>
       </c>
       <c r="C31">
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="D31" t="s">
-        <v>158</v>
+        <v>135</v>
       </c>
       <c r="E31">
         <v>20</v>
@@ -5632,13 +5620,13 @@
         <v>327</v>
       </c>
       <c r="C32">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="D32" t="s">
-        <v>158</v>
+        <v>135</v>
       </c>
       <c r="E32">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -5649,13 +5637,13 @@
         <v>329</v>
       </c>
       <c r="C33">
-        <v>100</v>
+        <v>300</v>
       </c>
       <c r="D33" t="s">
         <v>135</v>
       </c>
       <c r="E33">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -5666,13 +5654,13 @@
         <v>331</v>
       </c>
       <c r="C34">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="D34" t="s">
         <v>135</v>
       </c>
       <c r="E34">
-        <v>15</v>
+        <v>30</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -5683,13 +5671,13 @@
         <v>333</v>
       </c>
       <c r="C35">
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="D35" t="s">
-        <v>135</v>
+        <v>171</v>
       </c>
       <c r="E35">
-        <v>25</v>
+        <v>40</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -5700,13 +5688,13 @@
         <v>335</v>
       </c>
       <c r="C36">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="D36" t="s">
-        <v>135</v>
+        <v>171</v>
       </c>
       <c r="E36">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -5717,13 +5705,13 @@
         <v>337</v>
       </c>
       <c r="C37">
-        <v>100</v>
+        <v>300</v>
       </c>
       <c r="D37" t="s">
         <v>171</v>
       </c>
       <c r="E37">
-        <v>40</v>
+        <v>30</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -5734,7 +5722,7 @@
         <v>339</v>
       </c>
       <c r="C38">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="D38" t="s">
         <v>171</v>
@@ -5751,27 +5739,27 @@
         <v>341</v>
       </c>
       <c r="C39">
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="D39" t="s">
-        <v>171</v>
+        <v>342</v>
       </c>
       <c r="E39">
-        <v>30</v>
+        <v>20</v>
       </c>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" t="s">
+        <v>343</v>
+      </c>
+      <c r="B40" t="s">
+        <v>344</v>
+      </c>
+      <c r="C40">
+        <v>200</v>
+      </c>
+      <c r="D40" t="s">
         <v>342</v>
-      </c>
-      <c r="B40" t="s">
-        <v>343</v>
-      </c>
-      <c r="C40">
-        <v>400</v>
-      </c>
-      <c r="D40" t="s">
-        <v>171</v>
       </c>
       <c r="E40">
         <v>25</v>
@@ -5779,19 +5767,19 @@
     </row>
     <row r="41" spans="1:5">
       <c r="A41" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="B41" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="C41">
-        <v>100</v>
+        <v>300</v>
       </c>
       <c r="D41" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="E41">
-        <v>20</v>
+        <v>30</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -5802,10 +5790,10 @@
         <v>348</v>
       </c>
       <c r="C42">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="D42" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="E42">
         <v>25</v>
@@ -5819,10 +5807,10 @@
         <v>350</v>
       </c>
       <c r="C43">
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="D43" t="s">
-        <v>346</v>
+        <v>56</v>
       </c>
       <c r="E43">
         <v>30</v>
@@ -5836,13 +5824,13 @@
         <v>352</v>
       </c>
       <c r="C44">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="D44" t="s">
-        <v>346</v>
+        <v>56</v>
       </c>
       <c r="E44">
-        <v>25</v>
+        <v>35</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -5853,13 +5841,13 @@
         <v>354</v>
       </c>
       <c r="C45">
-        <v>100</v>
+        <v>300</v>
       </c>
       <c r="D45" t="s">
         <v>56</v>
       </c>
       <c r="E45">
-        <v>30</v>
+        <v>20</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -5870,13 +5858,13 @@
         <v>356</v>
       </c>
       <c r="C46">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="D46" t="s">
         <v>56</v>
       </c>
       <c r="E46">
-        <v>35</v>
+        <v>25</v>
       </c>
     </row>
     <row r="47" spans="1:5">
@@ -5887,47 +5875,47 @@
         <v>358</v>
       </c>
       <c r="C47">
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="D47" t="s">
-        <v>56</v>
+        <v>359</v>
       </c>
       <c r="E47">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="48" spans="1:5">
       <c r="A48" t="s">
+        <v>360</v>
+      </c>
+      <c r="B48" t="s">
+        <v>361</v>
+      </c>
+      <c r="C48">
+        <v>200</v>
+      </c>
+      <c r="D48" t="s">
         <v>359</v>
       </c>
-      <c r="B48" t="s">
-        <v>360</v>
-      </c>
-      <c r="C48">
-        <v>400</v>
-      </c>
-      <c r="D48" t="s">
-        <v>56</v>
-      </c>
       <c r="E48">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="49" spans="1:5">
       <c r="A49" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="B49" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="C49">
-        <v>100</v>
+        <v>300</v>
       </c>
       <c r="D49" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="E49">
-        <v>15</v>
+        <v>30</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -5938,13 +5926,13 @@
         <v>365</v>
       </c>
       <c r="C50">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="D50" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="E50">
-        <v>20</v>
+        <v>35</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -5955,13 +5943,13 @@
         <v>367</v>
       </c>
       <c r="C51">
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="D51" t="s">
-        <v>363</v>
+        <v>186</v>
       </c>
       <c r="E51">
-        <v>30</v>
+        <v>20</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -5972,13 +5960,13 @@
         <v>369</v>
       </c>
       <c r="C52">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="D52" t="s">
-        <v>363</v>
+        <v>186</v>
       </c>
       <c r="E52">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="53" spans="1:5">
@@ -5989,13 +5977,13 @@
         <v>371</v>
       </c>
       <c r="C53">
-        <v>100</v>
+        <v>300</v>
       </c>
       <c r="D53" t="s">
         <v>186</v>
       </c>
       <c r="E53">
-        <v>20</v>
+        <v>35</v>
       </c>
     </row>
     <row r="54" spans="1:5">
@@ -6006,46 +5994,12 @@
         <v>373</v>
       </c>
       <c r="C54">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="D54" t="s">
         <v>186</v>
       </c>
       <c r="E54">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5">
-      <c r="A55" t="s">
-        <v>374</v>
-      </c>
-      <c r="B55" t="s">
-        <v>375</v>
-      </c>
-      <c r="C55">
-        <v>300</v>
-      </c>
-      <c r="D55" t="s">
-        <v>186</v>
-      </c>
-      <c r="E55">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5">
-      <c r="A56" t="s">
-        <v>376</v>
-      </c>
-      <c r="B56" t="s">
-        <v>377</v>
-      </c>
-      <c r="C56">
-        <v>400</v>
-      </c>
-      <c r="D56" t="s">
-        <v>186</v>
-      </c>
-      <c r="E56">
         <v>35</v>
       </c>
     </row>
@@ -6066,8 +6020,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:K150"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G51" sqref="G51"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G93" sqref="G93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -6086,31 +6040,31 @@
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1">
       <c r="A1" s="3" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>50</v>
@@ -6119,13 +6073,13 @@
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="2" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D2" s="2">
         <v>2</v>
@@ -6137,13 +6091,13 @@
         <v>54</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="I2" s="11" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>56</v>
@@ -6151,13 +6105,13 @@
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="2" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D3" s="2">
         <v>3</v>
@@ -6166,16 +6120,16 @@
         <v>6</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>56</v>
@@ -6183,13 +6137,13 @@
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="2" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D4" s="2">
         <v>2</v>
@@ -6201,13 +6155,13 @@
         <v>63</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>56</v>
@@ -6215,13 +6169,13 @@
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="2" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D5" s="2">
         <v>2</v>
@@ -6233,13 +6187,13 @@
         <v>65</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="J5" s="2" t="s">
         <v>56</v>
@@ -6247,13 +6201,13 @@
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="2" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D6" s="2">
         <v>2</v>
@@ -6265,13 +6219,13 @@
         <v>68</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="J6" s="2" t="s">
         <v>56</v>
@@ -6279,13 +6233,13 @@
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="2" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D7" s="2">
         <v>3</v>
@@ -6297,10 +6251,10 @@
         <v>63</v>
       </c>
       <c r="G7" s="11" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="H7" s="11" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="I7" s="11"/>
       <c r="J7" s="2" t="s">
@@ -6309,13 +6263,13 @@
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="2" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D8" s="2">
         <v>3</v>
@@ -6327,10 +6281,10 @@
         <v>72</v>
       </c>
       <c r="G8" s="11" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="H8" s="11" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="I8" s="11"/>
       <c r="J8" s="2" t="s">
@@ -6339,13 +6293,13 @@
     </row>
     <row r="9" spans="1:11">
       <c r="A9" s="2" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D9" s="2">
         <v>2</v>
@@ -6357,10 +6311,10 @@
         <v>74</v>
       </c>
       <c r="G9" s="11" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="H9" s="11" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="I9" s="11"/>
       <c r="J9" s="2" t="s">
@@ -6369,13 +6323,13 @@
     </row>
     <row r="10" spans="1:11">
       <c r="A10" s="2" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D10" s="2">
         <v>2</v>
@@ -6387,10 +6341,10 @@
         <v>76</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="H10" s="11" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="I10" s="11"/>
       <c r="J10" s="2" t="s">
@@ -6399,13 +6353,13 @@
     </row>
     <row r="11" spans="1:11">
       <c r="A11" s="2" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D11" s="2">
         <v>2</v>
@@ -6417,10 +6371,10 @@
         <v>78</v>
       </c>
       <c r="G11" s="11" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="H11" s="11" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="I11" s="11"/>
       <c r="J11" s="2" t="s">
@@ -6429,13 +6383,13 @@
     </row>
     <row r="12" spans="1:11">
       <c r="A12" s="2" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D12" s="2">
         <v>3</v>
@@ -6447,10 +6401,10 @@
         <v>61</v>
       </c>
       <c r="G12" s="11" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="H12" s="11" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="I12" s="11"/>
       <c r="J12" s="2" t="s">
@@ -6459,13 +6413,13 @@
     </row>
     <row r="13" spans="1:11">
       <c r="A13" s="2" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D13" s="2">
         <v>3</v>
@@ -6488,13 +6442,13 @@
     </row>
     <row r="14" spans="1:11">
       <c r="A14" s="2" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D14" s="2">
         <v>2</v>
@@ -6517,13 +6471,13 @@
     </row>
     <row r="15" spans="1:11">
       <c r="A15" s="2" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D15" s="2">
         <v>2</v>
@@ -6546,13 +6500,13 @@
     </row>
     <row r="16" spans="1:11">
       <c r="A16" s="2" t="s">
-        <v>636</v>
+        <v>632</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>568</v>
+        <v>564</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D16" s="2">
         <v>3</v>
@@ -6561,7 +6515,7 @@
         <v>14</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>569</v>
+        <v>565</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>304</v>
@@ -6575,13 +6529,13 @@
     </row>
     <row r="17" spans="1:10">
       <c r="A17" s="2" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="D17" s="2">
         <v>3</v>
@@ -6604,13 +6558,13 @@
     </row>
     <row r="18" spans="1:10">
       <c r="A18" s="2" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D18" s="2">
         <v>2</v>
@@ -6633,13 +6587,13 @@
     </row>
     <row r="19" spans="1:10">
       <c r="A19" s="2" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D19" s="2">
         <v>3</v>
@@ -6662,13 +6616,13 @@
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="2" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D20" s="2">
         <v>2</v>
@@ -6680,10 +6634,10 @@
         <v>91</v>
       </c>
       <c r="G20" s="11" t="s">
+        <v>310</v>
+      </c>
+      <c r="H20" s="11" t="s">
         <v>312</v>
-      </c>
-      <c r="H20" s="11" t="s">
-        <v>314</v>
       </c>
       <c r="J20" s="2" t="s">
         <v>82</v>
@@ -6691,13 +6645,13 @@
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="2" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D21" s="2">
         <v>2</v>
@@ -6709,10 +6663,10 @@
         <v>89</v>
       </c>
       <c r="G21" s="11" t="s">
+        <v>310</v>
+      </c>
+      <c r="H21" s="11" t="s">
         <v>312</v>
-      </c>
-      <c r="H21" s="11" t="s">
-        <v>314</v>
       </c>
       <c r="J21" s="2" t="s">
         <v>82</v>
@@ -6720,13 +6674,13 @@
     </row>
     <row r="22" spans="1:10">
       <c r="A22" s="2" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D22" s="2">
         <v>3</v>
@@ -6738,10 +6692,10 @@
         <v>93</v>
       </c>
       <c r="G22" s="11" t="s">
+        <v>310</v>
+      </c>
+      <c r="H22" s="11" t="s">
         <v>312</v>
-      </c>
-      <c r="H22" s="11" t="s">
-        <v>314</v>
       </c>
       <c r="J22" s="2" t="s">
         <v>82</v>
@@ -6749,13 +6703,13 @@
     </row>
     <row r="23" spans="1:10">
       <c r="A23" s="2" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D23" s="2">
         <v>3</v>
@@ -6767,10 +6721,10 @@
         <v>95</v>
       </c>
       <c r="G23" s="11" t="s">
+        <v>310</v>
+      </c>
+      <c r="H23" s="11" t="s">
         <v>312</v>
-      </c>
-      <c r="H23" s="11" t="s">
-        <v>314</v>
       </c>
       <c r="J23" s="2" t="s">
         <v>82</v>
@@ -6778,13 +6732,13 @@
     </row>
     <row r="24" spans="1:10">
       <c r="A24" s="2" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D24" s="2">
         <v>2</v>
@@ -6796,10 +6750,10 @@
         <v>95</v>
       </c>
       <c r="G24" s="11" t="s">
+        <v>310</v>
+      </c>
+      <c r="H24" s="11" t="s">
         <v>312</v>
-      </c>
-      <c r="H24" s="11" t="s">
-        <v>314</v>
       </c>
       <c r="J24" s="2" t="s">
         <v>82</v>
@@ -6807,13 +6761,13 @@
     </row>
     <row r="25" spans="1:10">
       <c r="A25" s="2" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D25" s="2">
         <v>2</v>
@@ -6825,10 +6779,10 @@
         <v>97</v>
       </c>
       <c r="G25" s="11" t="s">
+        <v>310</v>
+      </c>
+      <c r="H25" s="11" t="s">
         <v>312</v>
-      </c>
-      <c r="H25" s="11" t="s">
-        <v>314</v>
       </c>
       <c r="J25" s="2" t="s">
         <v>82</v>
@@ -6836,13 +6790,13 @@
     </row>
     <row r="26" spans="1:10">
       <c r="A26" s="2" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D26" s="2">
         <v>2</v>
@@ -6854,10 +6808,10 @@
         <v>99</v>
       </c>
       <c r="G26" s="11" t="s">
+        <v>310</v>
+      </c>
+      <c r="H26" s="11" t="s">
         <v>312</v>
-      </c>
-      <c r="H26" s="11" t="s">
-        <v>314</v>
       </c>
       <c r="J26" s="2" t="s">
         <v>82</v>
@@ -6865,13 +6819,13 @@
     </row>
     <row r="27" spans="1:10">
       <c r="A27" s="2" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D27" s="2">
         <v>2</v>
@@ -6883,13 +6837,13 @@
         <v>101</v>
       </c>
       <c r="G27" s="11" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="J27" s="2" t="s">
         <v>103</v>
@@ -6897,13 +6851,13 @@
     </row>
     <row r="28" spans="1:10">
       <c r="A28" s="2" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D28" s="2">
         <v>2</v>
@@ -6915,7 +6869,7 @@
         <v>61</v>
       </c>
       <c r="G28" s="11" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="J28" s="2" t="s">
         <v>103</v>
@@ -6923,13 +6877,13 @@
     </row>
     <row r="29" spans="1:10">
       <c r="A29" s="2" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D29" s="2">
         <v>2</v>
@@ -6941,7 +6895,7 @@
         <v>104</v>
       </c>
       <c r="G29" s="11" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="J29" s="2" t="s">
         <v>103</v>
@@ -6949,13 +6903,13 @@
     </row>
     <row r="30" spans="1:10">
       <c r="A30" s="2" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D30" s="2">
         <v>3</v>
@@ -6967,7 +6921,7 @@
         <v>104</v>
       </c>
       <c r="G30" s="11" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="J30" s="2" t="s">
         <v>103</v>
@@ -6975,13 +6929,13 @@
     </row>
     <row r="31" spans="1:10">
       <c r="A31" s="2" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D31" s="2">
         <v>2</v>
@@ -6993,7 +6947,7 @@
         <v>108</v>
       </c>
       <c r="G31" s="11" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="J31" s="2" t="s">
         <v>103</v>
@@ -7001,13 +6955,13 @@
     </row>
     <row r="32" spans="1:10">
       <c r="A32" s="2" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D32" s="2">
         <v>2</v>
@@ -7019,7 +6973,7 @@
         <v>54</v>
       </c>
       <c r="G32" s="11" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="J32" s="2" t="s">
         <v>103</v>
@@ -7027,13 +6981,13 @@
     </row>
     <row r="33" spans="1:10">
       <c r="A33" s="2" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D33" s="2">
         <v>2</v>
@@ -7045,7 +6999,7 @@
         <v>110</v>
       </c>
       <c r="G33" s="11" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="J33" s="2" t="s">
         <v>103</v>
@@ -7053,13 +7007,13 @@
     </row>
     <row r="34" spans="1:10">
       <c r="A34" s="2" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D34" s="2">
         <v>3</v>
@@ -7071,7 +7025,7 @@
         <v>106</v>
       </c>
       <c r="G34" s="11" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="J34" s="2" t="s">
         <v>103</v>
@@ -7079,13 +7033,13 @@
     </row>
     <row r="35" spans="1:10">
       <c r="A35" s="2" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D35" s="2">
         <v>2</v>
@@ -7097,7 +7051,7 @@
         <v>112</v>
       </c>
       <c r="G35" s="11" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="J35" s="2" t="s">
         <v>103</v>
@@ -7105,13 +7059,13 @@
     </row>
     <row r="36" spans="1:10">
       <c r="A36" s="2" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D36" s="2">
         <v>2</v>
@@ -7123,13 +7077,13 @@
         <v>114</v>
       </c>
       <c r="G36" s="11" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="H36" s="11" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="I36" s="11" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="J36" s="2" t="s">
         <v>103</v>
@@ -7137,13 +7091,13 @@
     </row>
     <row r="37" spans="1:10">
       <c r="A37" s="2" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D37" s="2">
         <v>2</v>
@@ -7155,13 +7109,13 @@
         <v>116</v>
       </c>
       <c r="G37" s="11" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="H37" s="11" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="I37" s="11" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="J37" s="2" t="s">
         <v>103</v>
@@ -7169,13 +7123,13 @@
     </row>
     <row r="38" spans="1:10">
       <c r="A38" s="2" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D38" s="2">
         <v>2</v>
@@ -7187,10 +7141,10 @@
         <v>118</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="J38" s="2" t="s">
         <v>120</v>
@@ -7198,13 +7152,13 @@
     </row>
     <row r="39" spans="1:10">
       <c r="A39" s="2" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D39" s="2">
         <v>3</v>
@@ -7216,7 +7170,7 @@
         <v>121</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="J39" s="2" t="s">
         <v>120</v>
@@ -7224,13 +7178,13 @@
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="2" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D40" s="2">
         <v>3</v>
@@ -7239,10 +7193,10 @@
         <v>14</v>
       </c>
       <c r="F40" s="12" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="J40" s="2" t="s">
         <v>120</v>
@@ -7250,13 +7204,13 @@
     </row>
     <row r="41" spans="1:10">
       <c r="A41" s="2" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D41" s="2">
         <v>2</v>
@@ -7268,7 +7222,7 @@
         <v>121</v>
       </c>
       <c r="G41" s="11" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="J41" s="2" t="s">
         <v>120</v>
@@ -7276,13 +7230,13 @@
     </row>
     <row r="42" spans="1:10">
       <c r="A42" s="2" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D42" s="2">
         <v>3</v>
@@ -7294,7 +7248,7 @@
         <v>123</v>
       </c>
       <c r="G42" s="11" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="J42" s="2" t="s">
         <v>120</v>
@@ -7302,13 +7256,13 @@
     </row>
     <row r="43" spans="1:10">
       <c r="A43" s="2" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D43" s="2">
         <v>3</v>
@@ -7320,7 +7274,7 @@
         <v>125</v>
       </c>
       <c r="G43" s="11" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="J43" s="2" t="s">
         <v>120</v>
@@ -7328,13 +7282,13 @@
     </row>
     <row r="44" spans="1:10">
       <c r="A44" s="2" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="D44" s="2">
         <v>3</v>
@@ -7346,7 +7300,7 @@
         <v>127</v>
       </c>
       <c r="G44" s="11" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="J44" s="2" t="s">
         <v>120</v>
@@ -7354,13 +7308,13 @@
     </row>
     <row r="45" spans="1:10">
       <c r="A45" s="2" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D45" s="2">
         <v>2</v>
@@ -7372,7 +7326,7 @@
         <v>121</v>
       </c>
       <c r="G45" s="11" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="J45" s="2" t="s">
         <v>120</v>
@@ -7380,13 +7334,13 @@
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="2" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="D46" s="2">
         <v>2</v>
@@ -7398,7 +7352,7 @@
         <v>129</v>
       </c>
       <c r="G46" s="11" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="J46" s="2" t="s">
         <v>120</v>
@@ -7406,13 +7360,13 @@
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="2" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D47" s="2">
         <v>2</v>
@@ -7424,7 +7378,7 @@
         <v>131</v>
       </c>
       <c r="G47" s="11" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="J47" s="2" t="s">
         <v>120</v>
@@ -7432,13 +7386,13 @@
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="2" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D48" s="2">
         <v>2</v>
@@ -7450,7 +7404,7 @@
         <v>136</v>
       </c>
       <c r="G48" s="11" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="J48" s="2" t="s">
         <v>135</v>
@@ -7458,13 +7412,13 @@
     </row>
     <row r="49" spans="1:10">
       <c r="A49" s="2" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D49" s="2">
         <v>2</v>
@@ -7476,13 +7430,13 @@
         <v>138</v>
       </c>
       <c r="G49" s="11" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="I49" s="2" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="J49" s="2" t="s">
         <v>135</v>
@@ -7490,13 +7444,13 @@
     </row>
     <row r="50" spans="1:10">
       <c r="A50" s="2" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D50" s="2">
         <v>2</v>
@@ -7505,16 +7459,16 @@
         <v>6</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
       <c r="G50" s="11" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="I50" s="2" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="J50" s="2" t="s">
         <v>135</v>
@@ -7522,13 +7476,13 @@
     </row>
     <row r="51" spans="1:10">
       <c r="A51" s="2" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D51" s="2">
         <v>2</v>
@@ -7540,13 +7494,13 @@
         <v>144</v>
       </c>
       <c r="G51" s="11" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="I51" s="11" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="J51" s="2" t="s">
         <v>135</v>
@@ -7554,13 +7508,13 @@
     </row>
     <row r="52" spans="1:10">
       <c r="A52" s="2" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D52" s="2">
         <v>3</v>
@@ -7572,7 +7526,7 @@
         <v>150</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="J52" s="2" t="s">
         <v>135</v>
@@ -7580,13 +7534,13 @@
     </row>
     <row r="53" spans="1:10">
       <c r="A53" s="2" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D53" s="2">
         <v>3</v>
@@ -7595,10 +7549,10 @@
         <v>6</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="G53" s="2" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="J53" s="2" t="s">
         <v>135</v>
@@ -7606,13 +7560,13 @@
     </row>
     <row r="54" spans="1:10">
       <c r="A54" s="2" t="s">
-        <v>652</v>
+        <v>648</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="D54" s="2">
         <v>3</v>
@@ -7621,7 +7575,7 @@
         <v>6</v>
       </c>
       <c r="G54" s="11" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="J54" s="2" t="s">
         <v>135</v>
@@ -7629,13 +7583,13 @@
     </row>
     <row r="55" spans="1:10">
       <c r="A55" s="2" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D55" s="2">
         <v>3</v>
@@ -7647,7 +7601,7 @@
         <v>148</v>
       </c>
       <c r="G55" s="11" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="J55" s="2" t="s">
         <v>135</v>
@@ -7655,13 +7609,13 @@
     </row>
     <row r="56" spans="1:10">
       <c r="A56" s="2" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D56" s="2">
         <v>3</v>
@@ -7673,7 +7627,7 @@
         <v>136</v>
       </c>
       <c r="G56" s="11" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="J56" s="2" t="s">
         <v>135</v>
@@ -7681,13 +7635,13 @@
     </row>
     <row r="57" spans="1:10">
       <c r="A57" s="2" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D57" s="2">
         <v>3</v>
@@ -7699,7 +7653,7 @@
         <v>148</v>
       </c>
       <c r="G57" s="11" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="J57" s="2" t="s">
         <v>135</v>
@@ -7707,13 +7661,13 @@
     </row>
     <row r="58" spans="1:10">
       <c r="A58" s="2" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D58" s="2">
         <v>3</v>
@@ -7725,7 +7679,7 @@
         <v>150</v>
       </c>
       <c r="G58" s="11" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="J58" s="2" t="s">
         <v>135</v>
@@ -7733,13 +7687,13 @@
     </row>
     <row r="59" spans="1:10">
       <c r="A59" s="2" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D59" s="2">
         <v>3</v>
@@ -7751,7 +7705,7 @@
         <v>152</v>
       </c>
       <c r="G59" s="11" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="J59" s="2" t="s">
         <v>135</v>
@@ -7759,13 +7713,13 @@
     </row>
     <row r="60" spans="1:10">
       <c r="A60" s="2" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D60" s="2">
         <v>3</v>
@@ -7777,7 +7731,7 @@
         <v>154</v>
       </c>
       <c r="G60" s="11" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="J60" s="2" t="s">
         <v>135</v>
@@ -7785,13 +7739,13 @@
     </row>
     <row r="61" spans="1:10">
       <c r="A61" s="2" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D61" s="2">
         <v>2</v>
@@ -7803,7 +7757,7 @@
         <v>159</v>
       </c>
       <c r="G61" s="11" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="J61" s="2" t="s">
         <v>158</v>
@@ -7811,13 +7765,13 @@
     </row>
     <row r="62" spans="1:10">
       <c r="A62" s="2" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D62" s="2">
         <v>2</v>
@@ -7829,7 +7783,7 @@
         <v>161</v>
       </c>
       <c r="G62" s="11" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="J62" s="2" t="s">
         <v>158</v>
@@ -7837,13 +7791,13 @@
     </row>
     <row r="63" spans="1:10">
       <c r="A63" s="2" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D63" s="2">
         <v>3</v>
@@ -7855,10 +7809,10 @@
         <v>163</v>
       </c>
       <c r="G63" s="11" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="H63" s="2" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="J63" s="2" t="s">
         <v>158</v>
@@ -7866,13 +7820,13 @@
     </row>
     <row r="64" spans="1:10">
       <c r="A64" s="2" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D64" s="2">
         <v>2</v>
@@ -7884,10 +7838,10 @@
         <v>165</v>
       </c>
       <c r="G64" s="11" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="H64" s="2" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="J64" s="2" t="s">
         <v>158</v>
@@ -7895,13 +7849,13 @@
     </row>
     <row r="65" spans="1:10">
       <c r="A65" s="2" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="D65" s="2">
         <v>3</v>
@@ -7910,7 +7864,7 @@
         <v>6</v>
       </c>
       <c r="G65" s="11" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="J65" s="2" t="s">
         <v>158</v>
@@ -7918,13 +7872,13 @@
     </row>
     <row r="66" spans="1:10">
       <c r="A66" s="2" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>516</v>
+        <v>512</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D66" s="2">
         <v>3</v>
@@ -7936,7 +7890,7 @@
         <v>142</v>
       </c>
       <c r="G66" s="11" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="J66" s="2" t="s">
         <v>158</v>
@@ -7944,13 +7898,13 @@
     </row>
     <row r="67" spans="1:10">
       <c r="A67" s="2" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D67" s="2">
         <v>3</v>
@@ -7962,7 +7916,7 @@
         <v>140</v>
       </c>
       <c r="G67" s="11" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="J67" s="2" t="s">
         <v>158</v>
@@ -7970,13 +7924,13 @@
     </row>
     <row r="68" spans="1:10">
       <c r="A68" s="2" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D68" s="2">
         <v>3</v>
@@ -7988,7 +7942,7 @@
         <v>167</v>
       </c>
       <c r="G68" s="11" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="J68" s="2" t="s">
         <v>158</v>
@@ -7996,13 +7950,13 @@
     </row>
     <row r="69" spans="1:10">
       <c r="A69" s="2" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D69" s="2">
         <v>2</v>
@@ -8014,7 +7968,7 @@
         <v>140</v>
       </c>
       <c r="G69" s="11" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="J69" s="2" t="s">
         <v>158</v>
@@ -8022,13 +7976,13 @@
     </row>
     <row r="70" spans="1:10">
       <c r="A70" s="2" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D70" s="2">
         <v>2</v>
@@ -8040,7 +7994,7 @@
         <v>159</v>
       </c>
       <c r="G70" s="11" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="J70" s="2" t="s">
         <v>158</v>
@@ -8048,13 +8002,13 @@
     </row>
     <row r="71" spans="1:10">
       <c r="A71" s="2" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D71" s="2">
         <v>2</v>
@@ -8066,7 +8020,7 @@
         <v>165</v>
       </c>
       <c r="G71" s="11" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="J71" s="2" t="s">
         <v>158</v>
@@ -8074,13 +8028,13 @@
     </row>
     <row r="72" spans="1:10">
       <c r="A72" s="2" t="s">
-        <v>529</v>
+        <v>525</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>530</v>
+        <v>526</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D72" s="2">
         <v>3</v>
@@ -8092,7 +8046,7 @@
         <v>174</v>
       </c>
       <c r="G72" s="11" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="J72" s="2" t="s">
         <v>171</v>
@@ -8100,13 +8054,13 @@
     </row>
     <row r="73" spans="1:10">
       <c r="A73" s="2" t="s">
-        <v>531</v>
+        <v>527</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>532</v>
+        <v>528</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D73" s="2">
         <v>3</v>
@@ -8118,7 +8072,7 @@
         <v>176</v>
       </c>
       <c r="G73" s="2" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="J73" s="2" t="s">
         <v>171</v>
@@ -8126,13 +8080,13 @@
     </row>
     <row r="74" spans="1:10">
       <c r="A74" s="2" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>534</v>
+        <v>530</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D74" s="2">
         <v>3</v>
@@ -8144,7 +8098,7 @@
         <v>178</v>
       </c>
       <c r="G74" s="2" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="J74" s="2" t="s">
         <v>171</v>
@@ -8152,13 +8106,13 @@
     </row>
     <row r="75" spans="1:10">
       <c r="A75" s="2" t="s">
-        <v>535</v>
+        <v>531</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>536</v>
+        <v>532</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D75" s="2">
         <v>3</v>
@@ -8170,7 +8124,7 @@
         <v>180</v>
       </c>
       <c r="G75" s="2" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="J75" s="2" t="s">
         <v>171</v>
@@ -8178,13 +8132,13 @@
     </row>
     <row r="76" spans="1:10">
       <c r="A76" s="2" t="s">
-        <v>537</v>
+        <v>533</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D76" s="2">
         <v>3</v>
@@ -8196,7 +8150,7 @@
         <v>182</v>
       </c>
       <c r="G76" s="2" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="J76" s="2" t="s">
         <v>171</v>
@@ -8204,13 +8158,13 @@
     </row>
     <row r="77" spans="1:10">
       <c r="A77" s="2" t="s">
-        <v>539</v>
+        <v>535</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>540</v>
+        <v>536</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D77" s="2">
         <v>3</v>
@@ -8222,7 +8176,7 @@
         <v>191</v>
       </c>
       <c r="G77" s="2" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="J77" s="2" t="s">
         <v>186</v>
@@ -8230,13 +8184,13 @@
     </row>
     <row r="78" spans="1:10">
       <c r="A78" s="2" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>542</v>
+        <v>538</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D78" s="2">
         <v>3</v>
@@ -8248,7 +8202,7 @@
         <v>165</v>
       </c>
       <c r="G78" s="11" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="J78" s="2" t="s">
         <v>186</v>
@@ -8256,13 +8210,13 @@
     </row>
     <row r="79" spans="1:10">
       <c r="A79" s="2" t="s">
-        <v>543</v>
+        <v>539</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>544</v>
+        <v>540</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D79" s="2">
         <v>3</v>
@@ -8274,7 +8228,7 @@
         <v>163</v>
       </c>
       <c r="G79" s="11" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="J79" s="2" t="s">
         <v>186</v>
@@ -8282,13 +8236,13 @@
     </row>
     <row r="80" spans="1:10">
       <c r="A80" s="2" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D80" s="2">
         <v>3</v>
@@ -8300,7 +8254,7 @@
         <v>191</v>
       </c>
       <c r="G80" s="11" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="J80" s="2" t="s">
         <v>186</v>
@@ -8308,13 +8262,13 @@
     </row>
     <row r="81" spans="1:10">
       <c r="A81" s="2" t="s">
-        <v>547</v>
+        <v>543</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>548</v>
+        <v>544</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D81" s="2">
         <v>3</v>
@@ -8326,7 +8280,7 @@
         <v>161</v>
       </c>
       <c r="G81" s="11" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="J81" s="2" t="s">
         <v>186</v>
@@ -8334,13 +8288,13 @@
     </row>
     <row r="82" spans="1:10">
       <c r="A82" s="2" t="s">
-        <v>549</v>
+        <v>545</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D82" s="2">
         <v>3</v>
@@ -8352,7 +8306,7 @@
         <v>195</v>
       </c>
       <c r="G82" s="11" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="J82" s="2" t="s">
         <v>186</v>
@@ -8360,13 +8314,13 @@
     </row>
     <row r="83" spans="1:10">
       <c r="A83" s="2" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>552</v>
+        <v>548</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D83" s="2">
         <v>3</v>
@@ -8378,7 +8332,7 @@
         <v>197</v>
       </c>
       <c r="G83" s="11" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="J83" s="2" t="s">
         <v>186</v>
@@ -8386,13 +8340,13 @@
     </row>
     <row r="84" spans="1:10">
       <c r="A84" s="2" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D84" s="2">
         <v>3</v>
@@ -8404,24 +8358,22 @@
         <v>201</v>
       </c>
       <c r="G84" s="11" t="s">
-        <v>316</v>
-      </c>
-      <c r="H84" s="11" t="s">
-        <v>318</v>
-      </c>
+        <v>314</v>
+      </c>
+      <c r="H84" s="11"/>
       <c r="J84" s="2" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="85" spans="1:10">
       <c r="A85" s="2" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D85" s="2">
         <v>3</v>
@@ -8433,24 +8385,22 @@
         <v>203</v>
       </c>
       <c r="G85" s="11" t="s">
-        <v>316</v>
-      </c>
-      <c r="H85" s="11" t="s">
-        <v>318</v>
-      </c>
+        <v>314</v>
+      </c>
+      <c r="H85" s="11"/>
       <c r="J85" s="2" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="86" spans="1:10">
       <c r="A86" s="2" t="s">
-        <v>557</v>
+        <v>553</v>
       </c>
       <c r="B86" s="2" t="s">
         <v>213</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D86" s="2">
         <v>3</v>
@@ -8462,24 +8412,22 @@
         <v>205</v>
       </c>
       <c r="G86" s="11" t="s">
-        <v>316</v>
-      </c>
-      <c r="H86" s="11" t="s">
-        <v>318</v>
-      </c>
+        <v>314</v>
+      </c>
+      <c r="H86" s="11"/>
       <c r="J86" s="2" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="87" spans="1:10">
       <c r="A87" s="2" t="s">
-        <v>558</v>
+        <v>554</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D87" s="2">
         <v>2</v>
@@ -8491,24 +8439,22 @@
         <v>91</v>
       </c>
       <c r="G87" s="11" t="s">
-        <v>316</v>
-      </c>
-      <c r="H87" s="11" t="s">
-        <v>318</v>
-      </c>
+        <v>314</v>
+      </c>
+      <c r="H87" s="11"/>
       <c r="J87" s="2" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="88" spans="1:10">
       <c r="A88" s="2" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>561</v>
+        <v>557</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D88" s="2">
         <v>3</v>
@@ -8520,24 +8466,22 @@
         <v>89</v>
       </c>
       <c r="G88" s="11" t="s">
-        <v>316</v>
-      </c>
-      <c r="H88" s="11" t="s">
-        <v>318</v>
-      </c>
+        <v>314</v>
+      </c>
+      <c r="H88" s="11"/>
       <c r="J88" s="2" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="89" spans="1:10">
       <c r="A89" s="2" t="s">
-        <v>562</v>
+        <v>558</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D89" s="2">
         <v>3</v>
@@ -8546,27 +8490,25 @@
         <v>6</v>
       </c>
       <c r="F89" s="2" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
       <c r="G89" s="11" t="s">
-        <v>316</v>
-      </c>
-      <c r="H89" s="11" t="s">
-        <v>318</v>
-      </c>
+        <v>314</v>
+      </c>
+      <c r="H89" s="11"/>
       <c r="J89" s="2" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="90" spans="1:10">
       <c r="A90" s="2" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>566</v>
+        <v>562</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D90" s="2">
         <v>3</v>
@@ -8578,24 +8520,22 @@
         <v>205</v>
       </c>
       <c r="G90" s="11" t="s">
-        <v>316</v>
-      </c>
-      <c r="H90" s="11" t="s">
-        <v>318</v>
-      </c>
+        <v>314</v>
+      </c>
+      <c r="H90" s="11"/>
       <c r="J90" s="2" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="91" spans="1:10">
       <c r="A91" s="2" t="s">
-        <v>567</v>
+        <v>563</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>568</v>
+        <v>564</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D91" s="2">
         <v>3</v>
@@ -8604,7 +8544,7 @@
         <v>14</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>569</v>
+        <v>565</v>
       </c>
       <c r="G91" s="2" t="s">
         <v>296</v>
@@ -8615,13 +8555,13 @@
     </row>
     <row r="92" spans="1:10">
       <c r="A92" s="2" t="s">
-        <v>570</v>
+        <v>566</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>571</v>
+        <v>567</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D92" s="2">
         <v>2</v>
@@ -8641,13 +8581,13 @@
     </row>
     <row r="93" spans="1:10">
       <c r="A93" s="2" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D93" s="2">
         <v>2</v>
@@ -8667,13 +8607,13 @@
     </row>
     <row r="94" spans="1:10">
       <c r="A94" s="2" t="s">
-        <v>574</v>
+        <v>570</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>575</v>
+        <v>571</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D94" s="2">
         <v>3</v>
@@ -8693,13 +8633,13 @@
     </row>
     <row r="95" spans="1:10">
       <c r="A95" s="2" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>577</v>
+        <v>573</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D95" s="2">
         <v>2</v>
@@ -8719,13 +8659,13 @@
     </row>
     <row r="96" spans="1:10">
       <c r="A96" s="2" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>578</v>
+        <v>574</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D96" s="2">
         <v>2</v>
@@ -8742,13 +8682,13 @@
     </row>
     <row r="97" spans="1:10">
       <c r="A97" s="2" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>580</v>
+        <v>576</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D97" s="2">
         <v>1</v>
@@ -8774,13 +8714,13 @@
     </row>
     <row r="98" spans="1:10">
       <c r="A98" s="2" t="s">
-        <v>581</v>
+        <v>577</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D98" s="2">
         <v>2</v>
@@ -8806,13 +8746,13 @@
     </row>
     <row r="99" spans="1:10">
       <c r="A99" s="2" t="s">
-        <v>583</v>
+        <v>579</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>584</v>
+        <v>580</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D99" s="2">
         <v>2</v>
@@ -8838,13 +8778,13 @@
     </row>
     <row r="100" spans="1:10">
       <c r="A100" s="2" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>586</v>
+        <v>582</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="D100" s="2">
         <v>1</v>
@@ -8853,7 +8793,7 @@
         <v>12</v>
       </c>
       <c r="F100" s="2" t="s">
-        <v>587</v>
+        <v>583</v>
       </c>
       <c r="G100" s="2" t="s">
         <v>286</v>
@@ -8870,13 +8810,13 @@
     </row>
     <row r="101" spans="1:10">
       <c r="A101" s="2" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D101" s="2">
         <v>2</v>
@@ -8902,13 +8842,13 @@
     </row>
     <row r="102" spans="1:10">
       <c r="A102" s="2" t="s">
-        <v>589</v>
+        <v>585</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>590</v>
+        <v>586</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D102" s="2">
         <v>2</v>
@@ -8917,7 +8857,7 @@
         <v>6</v>
       </c>
       <c r="F102" s="2" t="s">
-        <v>591</v>
+        <v>587</v>
       </c>
       <c r="G102" s="2" t="s">
         <v>265</v>
@@ -8928,13 +8868,13 @@
     </row>
     <row r="103" spans="1:10">
       <c r="A103" s="2" t="s">
-        <v>592</v>
+        <v>588</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>593</v>
+        <v>589</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D103" s="2">
         <v>2</v>
@@ -8954,13 +8894,13 @@
     </row>
     <row r="104" spans="1:10">
       <c r="A104" s="2" t="s">
-        <v>594</v>
+        <v>590</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>595</v>
+        <v>591</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D104" s="2">
         <v>2</v>
@@ -8980,13 +8920,13 @@
     </row>
     <row r="105" spans="1:10">
       <c r="A105" s="2" t="s">
-        <v>596</v>
+        <v>592</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>597</v>
+        <v>593</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D105" s="2">
         <v>3</v>
@@ -9006,13 +8946,13 @@
     </row>
     <row r="106" spans="1:10">
       <c r="A106" s="2" t="s">
-        <v>598</v>
+        <v>594</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>599</v>
+        <v>595</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D106" s="2">
         <v>2</v>
@@ -9032,13 +8972,13 @@
     </row>
     <row r="107" spans="1:10">
       <c r="A107" s="2" t="s">
-        <v>600</v>
+        <v>596</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="D107" s="2">
         <v>2</v>
@@ -9047,7 +8987,7 @@
         <v>6</v>
       </c>
       <c r="F107" s="2" t="s">
-        <v>602</v>
+        <v>598</v>
       </c>
       <c r="G107" s="11" t="s">
         <v>272</v>
@@ -9058,13 +8998,13 @@
     </row>
     <row r="108" spans="1:10">
       <c r="A108" s="2" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D108" s="2">
         <v>2</v>
@@ -9084,13 +9024,13 @@
     </row>
     <row r="109" spans="1:10">
       <c r="A109" s="2" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>606</v>
+        <v>602</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D109" s="2">
         <v>2</v>
@@ -9107,13 +9047,13 @@
     </row>
     <row r="110" spans="1:10">
       <c r="A110" s="2" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>608</v>
+        <v>604</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="D110" s="2">
         <v>3</v>
@@ -9130,13 +9070,13 @@
     </row>
     <row r="111" spans="1:10">
       <c r="A111" s="2" t="s">
-        <v>609</v>
+        <v>605</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>610</v>
+        <v>606</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D111" s="2">
         <v>3</v>
@@ -9156,13 +9096,13 @@
     </row>
     <row r="112" spans="1:10">
       <c r="A112" s="2" t="s">
-        <v>611</v>
+        <v>607</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>612</v>
+        <v>608</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D112" s="2">
         <v>2</v>
@@ -9182,13 +9122,13 @@
     </row>
     <row r="113" spans="1:10">
       <c r="A113" s="2" t="s">
-        <v>613</v>
+        <v>609</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>614</v>
+        <v>610</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D113" s="2">
         <v>2</v>
@@ -9208,13 +9148,13 @@
     </row>
     <row r="114" spans="1:10">
       <c r="A114" s="2" t="s">
-        <v>615</v>
+        <v>611</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D114" s="2">
         <v>2</v>
@@ -9234,13 +9174,13 @@
     </row>
     <row r="115" spans="1:10">
       <c r="A115" s="2" t="s">
-        <v>616</v>
+        <v>612</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D115" s="2">
         <v>2</v>
@@ -9260,13 +9200,13 @@
     </row>
     <row r="116" spans="1:10">
       <c r="A116" s="2" t="s">
-        <v>618</v>
+        <v>614</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>619</v>
+        <v>615</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="D116" s="2">
         <v>3</v>
@@ -9283,13 +9223,13 @@
     </row>
     <row r="117" spans="1:10">
       <c r="A117" s="2" t="s">
-        <v>620</v>
+        <v>616</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>621</v>
+        <v>617</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D117" s="2">
         <v>2</v>
@@ -9309,13 +9249,13 @@
     </row>
     <row r="118" spans="1:10">
       <c r="A118" s="2" t="s">
-        <v>622</v>
+        <v>618</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>623</v>
+        <v>619</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D118" s="2">
         <v>3</v>
@@ -9335,13 +9275,13 @@
     </row>
     <row r="119" spans="1:10">
       <c r="A119" s="2" t="s">
-        <v>624</v>
+        <v>620</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>625</v>
+        <v>621</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D119" s="2">
         <v>2</v>
@@ -9361,13 +9301,13 @@
     </row>
     <row r="120" spans="1:10">
       <c r="A120" s="2" t="s">
-        <v>626</v>
+        <v>622</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>627</v>
+        <v>623</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D120" s="2">
         <v>2</v>

</xml_diff>